<commit_message>
Correct external curation status
</commit_message>
<xml_diff>
--- a/Population/BCIO_Population_Expanded.xlsx
+++ b/Population/BCIO_Population_Expanded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bgehrk/development/ontologies/Population/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50CBA41-1AAE-3D42-90D3-F71E010EBBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B37C1E-CF89-5143-977B-E1E55AE5617B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="740" windowWidth="14860" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8423,8 +8423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T845"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A796" workbookViewId="0">
-      <selection activeCell="A818" sqref="A818"/>
+    <sheetView tabSelected="1" topLeftCell="G810" workbookViewId="0">
+      <selection activeCell="P834" sqref="P834"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -37918,7 +37918,7 @@
         <v>1805</v>
       </c>
       <c r="O820" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="T820" t="s">
         <v>27</v>
@@ -38401,7 +38401,7 @@
         <v>1840</v>
       </c>
       <c r="O834" t="s">
-        <v>172</v>
+        <v>26</v>
       </c>
       <c r="T834" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Add new definition. Closes #1083
</commit_message>
<xml_diff>
--- a/Population/BCIO_Population_Expanded.xlsx
+++ b/Population/BCIO_Population_Expanded.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -9512,12 +9512,12 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>The aggregate of ability to comprehend spoken intervention language in a population.</t>
+          <t>A population statistic about ability to comprehend spoken intervention language.</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>linguistic capability  population statistic</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
@@ -9662,12 +9662,12 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>The aggregate of ability to read in intervention language in a population.</t>
+          <t>A population statistic about ability to read in intervention language.</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>linguistic capability  population statistic</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -9812,12 +9812,12 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>The aggregate of ability to speak in intervention language in a population.</t>
+          <t>A population statistic about ability to speak in intervention language.</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>linguistic capability  population statistic</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
@@ -9962,12 +9962,12 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>The aggregate of ability to write in intervention language in a population.</t>
+          <t>A population statistic about ability to write in intervention language.</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>linguistic capability  population statistic</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
@@ -10112,12 +10112,12 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>The aggregate of achieved bachelor's degree or equivalent level in a population.</t>
+          <t>A population statistic about achieved bachelor's degree or equivalent level.</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>highest level of formal educational qualification achieved population statistic</t>
         </is>
       </c>
       <c r="E246" t="inlineStr">
@@ -10262,12 +10262,12 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>The aggregate of achieved doctoral or equivalent level education in a population.</t>
+          <t>A population statistic about achieved doctoral or equivalent level education.</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>highest level of formal educational qualification achieved population statistic</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -10412,12 +10412,12 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>The aggregate of achieved early childhood education in a population.</t>
+          <t>A population statistic about achieved early childhood education.</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>highest level of formal educational qualification achieved population statistic</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
@@ -10562,12 +10562,12 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>The aggregate of achieved lower secondary education in a population.</t>
+          <t>A population statistic about achieved lower secondary education.</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>highest level of formal educational qualification achieved population statistic</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
@@ -10712,12 +10712,12 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>The aggregate of achieved master's or equivalent level in a population.</t>
+          <t>A population statistic about achieved master's or equivalent level.</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>highest level of formal educational qualification achieved population statistic</t>
         </is>
       </c>
       <c r="E258" t="inlineStr">
@@ -10862,12 +10862,12 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>The aggregate of achieved primary education in a population.</t>
+          <t>A population statistic about achieved primary education.</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>highest level of formal educational qualification achieved population statistic</t>
         </is>
       </c>
       <c r="E261" t="inlineStr">
@@ -11012,12 +11012,12 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>The aggregate of achieved upper secondary education  in a population.</t>
+          <t>A population statistic about achieved upper secondary education .</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>population statistic</t>
         </is>
       </c>
       <c r="E264" t="inlineStr">
@@ -11162,12 +11162,12 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive brother in a population.</t>
+          <t>A population statistic about adoptive brother.</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>adoptive sibling population statistic</t>
         </is>
       </c>
       <c r="E267" t="inlineStr">
@@ -11312,12 +11312,12 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive child in a population.</t>
+          <t>A population statistic about adoptive child.</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>child relation population statistic</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
@@ -11462,12 +11462,12 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive daughter in a population.</t>
+          <t>A population statistic about adoptive daughter.</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>adoptive child population statistic</t>
         </is>
       </c>
       <c r="E273" t="inlineStr">
@@ -11612,12 +11612,12 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive father in a population.</t>
+          <t>A population statistic about adoptive father.</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>adoptive parent population statistic</t>
         </is>
       </c>
       <c r="E276" t="inlineStr">
@@ -11762,12 +11762,12 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive mother in a population.</t>
+          <t>A population statistic about adoptive mother.</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>adoptive parent population statistic</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
@@ -11912,12 +11912,12 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive parent in a population.</t>
+          <t>A population statistic about adoptive parent.</t>
         </is>
       </c>
       <c r="D282" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>parent population statistic</t>
         </is>
       </c>
       <c r="E282" t="inlineStr">
@@ -12062,12 +12062,12 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive sibling in a population.</t>
+          <t>A population statistic about adoptive sibling.</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sibling population statistic</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
@@ -12212,12 +12212,12 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive sister in a population.</t>
+          <t>A population statistic about adoptive sister.</t>
         </is>
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>adoptive sibling population statistic</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
@@ -12362,12 +12362,12 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>The aggregate of adoptive son in a population.</t>
+          <t>A population statistic about adoptive son.</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>adoptive child population statistic</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
@@ -12512,12 +12512,12 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>The aggregate of adult in a population.</t>
+          <t>A population statistic about adult.</t>
         </is>
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
@@ -12662,12 +12662,12 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>The aggregate of agreed rent-free occupier in a population.</t>
+          <t>A population statistic about agreed rent-free occupier.</t>
         </is>
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>rent-free occupier population statistic</t>
         </is>
       </c>
       <c r="E297" t="inlineStr">
@@ -12812,12 +12812,12 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>The aggregate of asexual in a population.</t>
+          <t>A population statistic about asexual.</t>
         </is>
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sexual orientation population statistic</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
@@ -12962,12 +12962,12 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>The aggregate of aunt in a population.</t>
+          <t>A population statistic about aunt.</t>
         </is>
       </c>
       <c r="D303" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E303" t="inlineStr">
@@ -13112,12 +13112,12 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>The aggregate of biological brother in a population.</t>
+          <t>A population statistic about biological brother.</t>
         </is>
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological sibling population statistic</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -13262,12 +13262,12 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>The aggregate of biological child in a population.</t>
+          <t>A population statistic about biological child.</t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>child relation population statistic</t>
         </is>
       </c>
       <c r="E309" t="inlineStr">
@@ -13412,12 +13412,12 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>The aggregate of biological daughter in a population.</t>
+          <t>A population statistic about biological daughter.</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological child population statistic</t>
         </is>
       </c>
       <c r="E312" t="inlineStr">
@@ -13562,12 +13562,12 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>The aggregate of biological father in a population.</t>
+          <t>A population statistic about biological father.</t>
         </is>
       </c>
       <c r="D315" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological parent population statistic</t>
         </is>
       </c>
       <c r="E315" t="inlineStr">
@@ -13712,12 +13712,12 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>The aggregate of biological mother in a population.</t>
+          <t>A population statistic about biological mother.</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological parent population statistic</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
@@ -13862,12 +13862,12 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>The aggregate of biological parent in a population.</t>
+          <t>A population statistic about biological parent.</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>parent population statistic</t>
         </is>
       </c>
       <c r="E321" t="inlineStr">
@@ -14012,12 +14012,12 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>The aggregate of biological sex in a population.</t>
+          <t>A population statistic about biological sex.</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>bodily quality population statistic</t>
         </is>
       </c>
       <c r="E324" t="inlineStr">
@@ -14162,12 +14162,12 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>The aggregate of biological sibling in a population.</t>
+          <t>A population statistic about biological sibling.</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sibling population statistic</t>
         </is>
       </c>
       <c r="E327" t="inlineStr">
@@ -14312,12 +14312,12 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>The aggregate of biological sister in a population.</t>
+          <t>A population statistic about biological sister.</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological sibling population statistic</t>
         </is>
       </c>
       <c r="E330" t="inlineStr">
@@ -14462,12 +14462,12 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>The aggregate of biological son in a population.</t>
+          <t>A population statistic about biological son.</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological child population statistic</t>
         </is>
       </c>
       <c r="E333" t="inlineStr">
@@ -14612,12 +14612,12 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>The aggregate of bisexual in a population.</t>
+          <t>A population statistic about bisexual.</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sexual orientation population statistic</t>
         </is>
       </c>
       <c r="E336" t="inlineStr">
@@ -14762,12 +14762,12 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>The aggregate of caregiving role in a population.</t>
+          <t>A population statistic about caregiving role.</t>
         </is>
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>role population statistic</t>
         </is>
       </c>
       <c r="E339" t="inlineStr">
@@ -14912,12 +14912,12 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>The aggregate of caste membership in a population.</t>
+          <t>A population statistic about caste membership.</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E342" t="inlineStr">
@@ -15062,12 +15062,12 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>The aggregate of child in a population.</t>
+          <t>A population statistic about child.</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E345" t="inlineStr">
@@ -15212,12 +15212,12 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>The aggregate of child relation in a population.</t>
+          <t>A population statistic about child relation.</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E348" t="inlineStr">
@@ -15362,12 +15362,12 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>The aggregate of cisgender in a population.</t>
+          <t>A population statistic about cisgender.</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>gender identity population statistic</t>
         </is>
       </c>
       <c r="E351" t="inlineStr">
@@ -15512,12 +15512,12 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>The aggregate of country of birth in a population.</t>
+          <t>A population statistic about country of birth.</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>geographic location population statistic</t>
         </is>
       </c>
       <c r="E354" t="inlineStr">
@@ -15662,12 +15662,12 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>The aggregate of cousin in a population.</t>
+          <t>A population statistic about cousin.</t>
         </is>
       </c>
       <c r="D357" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E357" t="inlineStr">
@@ -15812,12 +15812,12 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>The aggregate of disabled in a population.</t>
+          <t>A population statistic about disabled.</t>
         </is>
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E360" t="inlineStr">
@@ -15962,12 +15962,12 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>The aggregate of discipline of current programme of study or training in a population.</t>
+          <t>A population statistic about discipline of current programme of study or training.</t>
         </is>
       </c>
       <c r="D363" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>expertise discipline population statistic</t>
         </is>
       </c>
       <c r="E363" t="inlineStr">
@@ -16112,12 +16112,12 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>The aggregate of discipline of highest level of formal educational qualification achieved in a population.</t>
+          <t>A population statistic about discipline of highest level of formal educational qualification achieved.</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>expertise discipline population statistic</t>
         </is>
       </c>
       <c r="E366" t="inlineStr">
@@ -16262,12 +16262,12 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>The aggregate of divorced or separated in a population.</t>
+          <t>A population statistic about divorced or separated.</t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>relationship status population statistic</t>
         </is>
       </c>
       <c r="E369" t="inlineStr">
@@ -16412,12 +16412,12 @@
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>The aggregate of doctoral student role in a population.</t>
+          <t>A population statistic about doctoral student role.</t>
         </is>
       </c>
       <c r="D372" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>higher education student role population statistic</t>
         </is>
       </c>
       <c r="E372" t="inlineStr">
@@ -16562,12 +16562,12 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>The aggregate of employed in a population.</t>
+          <t>A population statistic about employed.</t>
         </is>
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E375" t="inlineStr">
@@ -16712,12 +16712,12 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>The aggregate of employed full time in a population.</t>
+          <t>A population statistic about employed full time.</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E378" t="inlineStr">
@@ -16862,12 +16862,12 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>The aggregate of employed in shift work in a population.</t>
+          <t>A population statistic about employed in shift work.</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E381" t="inlineStr">
@@ -17012,12 +17012,12 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>The aggregate of employed part time in a population.</t>
+          <t>A population statistic about employed part time.</t>
         </is>
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E384" t="inlineStr">
@@ -17162,12 +17162,12 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>The aggregate of employment status in a population.</t>
+          <t>A population statistic about employment status.</t>
         </is>
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>quality population statistic</t>
         </is>
       </c>
       <c r="E387" t="inlineStr">
@@ -17312,12 +17312,12 @@
       </c>
       <c r="C390" t="inlineStr">
         <is>
-          <t>The aggregate of ethnic group membership in a population.</t>
+          <t>A population statistic about ethnic group membership.</t>
         </is>
       </c>
       <c r="D390" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>self-identity population statistic</t>
         </is>
       </c>
       <c r="E390" t="inlineStr">
@@ -17462,12 +17462,12 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>The aggregate of expertise discipline in a population.</t>
+          <t>A population statistic about expertise discipline.</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>specifically dependent continuant population statistic</t>
         </is>
       </c>
       <c r="E393" t="inlineStr">
@@ -17612,12 +17612,12 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>The aggregate of family member in a population.</t>
+          <t>A population statistic about family member.</t>
         </is>
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E396" t="inlineStr">
@@ -17762,12 +17762,12 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>The aggregate of father in a population.</t>
+          <t>A population statistic about father.</t>
         </is>
       </c>
       <c r="D399" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>parent population statistic</t>
         </is>
       </c>
       <c r="E399" t="inlineStr">
@@ -17912,12 +17912,12 @@
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>The aggregate of female biological sex in a population.</t>
+          <t>A population statistic about female biological sex.</t>
         </is>
       </c>
       <c r="D402" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological sex population statistic</t>
         </is>
       </c>
       <c r="E402" t="inlineStr">
@@ -18062,12 +18062,12 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>The aggregate of female gender in a population.</t>
+          <t>A population statistic about female gender.</t>
         </is>
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>gender identity population statistic</t>
         </is>
       </c>
       <c r="E405" t="inlineStr">
@@ -18212,12 +18212,12 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>The aggregate of foster brother in a population.</t>
+          <t>A population statistic about foster brother.</t>
         </is>
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>foster sibling population statistic</t>
         </is>
       </c>
       <c r="E408" t="inlineStr">
@@ -18362,12 +18362,12 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>The aggregate of foster child in a population.</t>
+          <t>A population statistic about foster child.</t>
         </is>
       </c>
       <c r="D411" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>child relation population statistic</t>
         </is>
       </c>
       <c r="E411" t="inlineStr">
@@ -18512,12 +18512,12 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>The aggregate of foster daughter in a population.</t>
+          <t>A population statistic about foster daughter.</t>
         </is>
       </c>
       <c r="D414" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>foster child population statistic</t>
         </is>
       </c>
       <c r="E414" t="inlineStr">
@@ -18662,12 +18662,12 @@
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>The aggregate of foster father in a population.</t>
+          <t>A population statistic about foster father.</t>
         </is>
       </c>
       <c r="D417" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>foster parent population statistic</t>
         </is>
       </c>
       <c r="E417" t="inlineStr">
@@ -18812,12 +18812,12 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>The aggregate of foster mother in a population.</t>
+          <t>A population statistic about foster mother.</t>
         </is>
       </c>
       <c r="D420" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>foster parent population statistic</t>
         </is>
       </c>
       <c r="E420" t="inlineStr">
@@ -18962,12 +18962,12 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>The aggregate of foster parent in a population.</t>
+          <t>A population statistic about foster parent.</t>
         </is>
       </c>
       <c r="D423" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>parent population statistic</t>
         </is>
       </c>
       <c r="E423" t="inlineStr">
@@ -19112,12 +19112,12 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>The aggregate of foster sibling in a population.</t>
+          <t>A population statistic about foster sibling.</t>
         </is>
       </c>
       <c r="D426" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sibling population statistic</t>
         </is>
       </c>
       <c r="E426" t="inlineStr">
@@ -19262,12 +19262,12 @@
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>The aggregate of foster sister in a population.</t>
+          <t>A population statistic about foster sister.</t>
         </is>
       </c>
       <c r="D429" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>foster sibling population statistic</t>
         </is>
       </c>
       <c r="E429" t="inlineStr">
@@ -19412,12 +19412,12 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>The aggregate of foster son in a population.</t>
+          <t>A population statistic about foster son.</t>
         </is>
       </c>
       <c r="D432" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>foster child population statistic</t>
         </is>
       </c>
       <c r="E432" t="inlineStr">
@@ -19562,12 +19562,12 @@
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>The aggregate of gender identity in a population.</t>
+          <t>A population statistic about gender identity.</t>
         </is>
       </c>
       <c r="D435" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>self-identity population statistic</t>
         </is>
       </c>
       <c r="E435" t="inlineStr">
@@ -19712,12 +19712,12 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>The aggregate of graduate student role in a population.</t>
+          <t>A population statistic about graduate student role.</t>
         </is>
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>higher education student role population statistic</t>
         </is>
       </c>
       <c r="E438" t="inlineStr">
@@ -19862,12 +19862,12 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>The aggregate of grandfather in a population.</t>
+          <t>A population statistic about grandfather.</t>
         </is>
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>grandparent population statistic</t>
         </is>
       </c>
       <c r="E441" t="inlineStr">
@@ -20012,12 +20012,12 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>The aggregate of grandmother in a population.</t>
+          <t>A population statistic about grandmother.</t>
         </is>
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>grandparent population statistic</t>
         </is>
       </c>
       <c r="E444" t="inlineStr">
@@ -20162,12 +20162,12 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>The aggregate of grandparent in a population.</t>
+          <t>A population statistic about grandparent.</t>
         </is>
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E447" t="inlineStr">
@@ -20312,12 +20312,12 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>The aggregate of having enacted a behaviour in a population.</t>
+          <t>A population statistic about having enacted a behaviour.</t>
         </is>
       </c>
       <c r="D450" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E450" t="inlineStr">
@@ -20462,12 +20462,12 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>The aggregate of health insurance policy holder role in a population.</t>
+          <t>A population statistic about health insurance policy holder role.</t>
         </is>
       </c>
       <c r="D453" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>policy holder role population statistic</t>
         </is>
       </c>
       <c r="E453" t="inlineStr">
@@ -20612,12 +20612,12 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>The aggregate of health status attribute in a population.</t>
+          <t>A population statistic about health status attribute.</t>
         </is>
       </c>
       <c r="D456" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E456" t="inlineStr">
@@ -20762,12 +20762,12 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>The aggregate of heterosexual in a population.</t>
+          <t>A population statistic about heterosexual.</t>
         </is>
       </c>
       <c r="D459" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sexual orientation population statistic</t>
         </is>
       </c>
       <c r="E459" t="inlineStr">
@@ -20912,12 +20912,12 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>The aggregate of higher education student role in a population.</t>
+          <t>A population statistic about higher education student role.</t>
         </is>
       </c>
       <c r="D462" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>student or trainee role population statistic</t>
         </is>
       </c>
       <c r="E462" t="inlineStr">
@@ -21062,12 +21062,12 @@
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>The aggregate of highest level of formal educational qualification achieved in a population.</t>
+          <t>A population statistic about highest level of formal educational qualification achieved.</t>
         </is>
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
@@ -21212,12 +21212,12 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>The aggregate of history of exposure to an occupational hazard in a population.</t>
+          <t>A population statistic about history of exposure to an occupational hazard.</t>
         </is>
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -21362,12 +21362,12 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>The aggregate of history of exposure to childhood maltreatment in a population.</t>
+          <t>A population statistic about history of exposure to childhood maltreatment.</t>
         </is>
       </c>
       <c r="D471" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E471" t="inlineStr">
@@ -21512,12 +21512,12 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>The aggregate of homeless person in a population.</t>
+          <t>A population statistic about homeless person.</t>
         </is>
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E474" t="inlineStr">
@@ -21662,12 +21662,12 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>The aggregate of homemaker status in a population.</t>
+          <t>A population statistic about homemaker status.</t>
         </is>
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E477" t="inlineStr">
@@ -21812,12 +21812,12 @@
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>The aggregate of homosexual in a population.</t>
+          <t>A population statistic about homosexual.</t>
         </is>
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sexual orientation population statistic</t>
         </is>
       </c>
       <c r="E480" t="inlineStr">
@@ -21962,12 +21962,12 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>The aggregate of household income in a population.</t>
+          <t>A population statistic about household income.</t>
         </is>
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>object aggregate population statistic</t>
         </is>
       </c>
       <c r="E483" t="inlineStr">
@@ -22312,12 +22312,12 @@
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>The aggregate of human age in a population.</t>
+          <t>A population statistic about human age.</t>
         </is>
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E490" t="inlineStr">
@@ -22562,12 +22562,12 @@
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>The aggregate of immigrant in a population.</t>
+          <t>A population statistic about immigrant.</t>
         </is>
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E495" t="inlineStr">
@@ -22712,12 +22712,12 @@
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>The aggregate of in a legal marriage or union in a population.</t>
+          <t>A population statistic about in a legal marriage or union.</t>
         </is>
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>relationship status population statistic</t>
         </is>
       </c>
       <c r="E498" t="inlineStr">
@@ -22862,12 +22862,12 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>The aggregate of in a stable or common law relationship in a population.</t>
+          <t>A population statistic about in a stable or common law relationship.</t>
         </is>
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>relationship status population statistic</t>
         </is>
       </c>
       <c r="E501" t="inlineStr">
@@ -23012,12 +23012,12 @@
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>The aggregate of in permanent employment in a population.</t>
+          <t>A population statistic about in permanent employment.</t>
         </is>
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E504" t="inlineStr">
@@ -23162,12 +23162,12 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>The aggregate of in short term or temporary employment with known conditions in a population.</t>
+          <t>A population statistic about in short term or temporary employment with known conditions.</t>
         </is>
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E507" t="inlineStr">
@@ -23312,12 +23312,12 @@
       </c>
       <c r="C510" t="inlineStr">
         <is>
-          <t>The aggregate of in uncertain employment in a population.</t>
+          <t>A population statistic about in uncertain employment.</t>
         </is>
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E510" t="inlineStr">
@@ -23462,12 +23462,12 @@
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>The aggregate of income-related welfare benefit in a population.</t>
+          <t>A population statistic about income-related welfare benefit.</t>
         </is>
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>individual income population statistic</t>
         </is>
       </c>
       <c r="E513" t="inlineStr">
@@ -23612,12 +23612,12 @@
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>The aggregate of independently wealthy status in a population.</t>
+          <t>A population statistic about independently wealthy status.</t>
         </is>
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E516" t="inlineStr">
@@ -23762,12 +23762,12 @@
       </c>
       <c r="C519" t="inlineStr">
         <is>
-          <t>The aggregate of individual human behaviour in a population.</t>
+          <t>A population statistic about individual human behaviour.</t>
         </is>
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>bodily process population statistic</t>
         </is>
       </c>
       <c r="E519" t="inlineStr">
@@ -24112,12 +24112,12 @@
       </c>
       <c r="C526" t="inlineStr">
         <is>
-          <t>The aggregate of individual income in a population.</t>
+          <t>A population statistic about individual income.</t>
         </is>
       </c>
       <c r="D526" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E526" t="inlineStr">
@@ -24462,12 +24462,12 @@
       </c>
       <c r="C533" t="inlineStr">
         <is>
-          <t>The aggregate of influencer role in a population.</t>
+          <t>A population statistic about influencer role.</t>
         </is>
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>social role population statistic</t>
         </is>
       </c>
       <c r="E533" t="inlineStr">
@@ -24612,12 +24612,12 @@
       </c>
       <c r="C536" t="inlineStr">
         <is>
-          <t>The aggregate of informal education student role in a population.</t>
+          <t>A population statistic about informal education student role.</t>
         </is>
       </c>
       <c r="D536" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>student or trainee role population statistic</t>
         </is>
       </c>
       <c r="E536" t="inlineStr">
@@ -24762,12 +24762,12 @@
       </c>
       <c r="C539" t="inlineStr">
         <is>
-          <t>The aggregate of inpatient role in a population.</t>
+          <t>A population statistic about inpatient role.</t>
         </is>
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>patient role population statistic</t>
         </is>
       </c>
       <c r="E539" t="inlineStr">
@@ -24912,12 +24912,12 @@
       </c>
       <c r="C542" t="inlineStr">
         <is>
-          <t>The aggregate of insured party role in a population.</t>
+          <t>A population statistic about insured party role.</t>
         </is>
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>role population statistic</t>
         </is>
       </c>
       <c r="E542" t="inlineStr">
@@ -25062,12 +25062,12 @@
       </c>
       <c r="C545" t="inlineStr">
         <is>
-          <t>The aggregate of interpersonal role in a population.</t>
+          <t>A population statistic about interpersonal role.</t>
         </is>
       </c>
       <c r="D545" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>role population statistic</t>
         </is>
       </c>
       <c r="E545" t="inlineStr">
@@ -25212,12 +25212,12 @@
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>The aggregate of language proficiency in a population.</t>
+          <t>A population statistic about language proficiency.</t>
         </is>
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>linguistic capability  population statistic</t>
         </is>
       </c>
       <c r="E548" t="inlineStr">
@@ -25562,12 +25562,12 @@
       </c>
       <c r="C555" t="inlineStr">
         <is>
-          <t>The aggregate of linguistic capability in a population.</t>
+          <t>A population statistic about linguistic capability.</t>
         </is>
       </c>
       <c r="D555" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>mental capability population statistic</t>
         </is>
       </c>
       <c r="E555" t="inlineStr">
@@ -25912,12 +25912,12 @@
       </c>
       <c r="C562" t="inlineStr">
         <is>
-          <t>The aggregate of long-term disabled in a population.</t>
+          <t>A population statistic about long-term disabled.</t>
         </is>
       </c>
       <c r="D562" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>disabled population statistic</t>
         </is>
       </c>
       <c r="E562" t="inlineStr">
@@ -26062,12 +26062,12 @@
       </c>
       <c r="C565" t="inlineStr">
         <is>
-          <t>The aggregate of male biological sex in a population.</t>
+          <t>A population statistic about male biological sex.</t>
         </is>
       </c>
       <c r="D565" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>biological sex population statistic</t>
         </is>
       </c>
       <c r="E565" t="inlineStr">
@@ -26212,12 +26212,12 @@
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>The aggregate of male gender in a population.</t>
+          <t>A population statistic about male gender.</t>
         </is>
       </c>
       <c r="D568" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>gender identity population statistic</t>
         </is>
       </c>
       <c r="E568" t="inlineStr">
@@ -26362,12 +26362,12 @@
       </c>
       <c r="C571" t="inlineStr">
         <is>
-          <t>The aggregate of masters student role in a population.</t>
+          <t>A population statistic about masters student role.</t>
         </is>
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>higher education student role population statistic</t>
         </is>
       </c>
       <c r="E571" t="inlineStr">
@@ -26512,12 +26512,12 @@
       </c>
       <c r="C574" t="inlineStr">
         <is>
-          <t>The aggregate of medication use status in a population.</t>
+          <t>A population statistic about medication use status.</t>
         </is>
       </c>
       <c r="D574" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>health status attribute population statistic</t>
         </is>
       </c>
       <c r="E574" t="inlineStr">
@@ -26662,12 +26662,12 @@
       </c>
       <c r="C577" t="inlineStr">
         <is>
-          <t>The aggregate of member of a multi-person household in a population.</t>
+          <t>A population statistic about member of a multi-person household.</t>
         </is>
       </c>
       <c r="D577" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E577" t="inlineStr">
@@ -26812,12 +26812,12 @@
       </c>
       <c r="C580" t="inlineStr">
         <is>
-          <t>The aggregate of member of a multi-person household all related in a population.</t>
+          <t>A population statistic about member of a multi-person household all related.</t>
         </is>
       </c>
       <c r="D580" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>member of a multi-person household population statistic</t>
         </is>
       </c>
       <c r="E580" t="inlineStr">
@@ -26962,12 +26962,12 @@
       </c>
       <c r="C583" t="inlineStr">
         <is>
-          <t>The aggregate of member of a multi-person household not related in a population.</t>
+          <t>A population statistic about member of a multi-person household not related.</t>
         </is>
       </c>
       <c r="D583" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>member of a multi-person household population statistic</t>
         </is>
       </c>
       <c r="E583" t="inlineStr">
@@ -27112,12 +27112,12 @@
       </c>
       <c r="C586" t="inlineStr">
         <is>
-          <t>The aggregate of member of a multi-person household some related in a population.</t>
+          <t>A population statistic about member of a multi-person household some related.</t>
         </is>
       </c>
       <c r="D586" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>member of a multi-person household population statistic</t>
         </is>
       </c>
       <c r="E586" t="inlineStr">
@@ -27262,12 +27262,12 @@
       </c>
       <c r="C589" t="inlineStr">
         <is>
-          <t>The aggregate of member of a multi-person multi-generational household in a population.</t>
+          <t>A population statistic about member of a multi-person multi-generational household.</t>
         </is>
       </c>
       <c r="D589" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>member of a multi-person household population statistic</t>
         </is>
       </c>
       <c r="E589" t="inlineStr">
@@ -27412,12 +27412,12 @@
       </c>
       <c r="C592" t="inlineStr">
         <is>
-          <t>The aggregate of member of a one person household in a population.</t>
+          <t>A population statistic about member of a one person household.</t>
         </is>
       </c>
       <c r="D592" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E592" t="inlineStr">
@@ -27562,12 +27562,12 @@
       </c>
       <c r="C595" t="inlineStr">
         <is>
-          <t>The aggregate of mental capability in a population.</t>
+          <t>A population statistic about mental capability.</t>
         </is>
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal capability population statistic</t>
         </is>
       </c>
       <c r="E595" t="inlineStr">
@@ -27912,12 +27912,12 @@
       </c>
       <c r="C602" t="inlineStr">
         <is>
-          <t>The aggregate of mother in a population.</t>
+          <t>A population statistic about mother.</t>
         </is>
       </c>
       <c r="D602" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>parent population statistic</t>
         </is>
       </c>
       <c r="E602" t="inlineStr">
@@ -28062,12 +28062,12 @@
       </c>
       <c r="C605" t="inlineStr">
         <is>
-          <t>The aggregate of nephew in a population.</t>
+          <t>A population statistic about nephew.</t>
         </is>
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E605" t="inlineStr">
@@ -28212,12 +28212,12 @@
       </c>
       <c r="C608" t="inlineStr">
         <is>
-          <t>The aggregate of niece in a population.</t>
+          <t>A population statistic about niece.</t>
         </is>
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E608" t="inlineStr">
@@ -28362,12 +28362,12 @@
       </c>
       <c r="C611" t="inlineStr">
         <is>
-          <t>The aggregate of non-gendered identity in a population.</t>
+          <t>A population statistic about non-gendered identity.</t>
         </is>
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>self-identity population statistic</t>
         </is>
       </c>
       <c r="E611" t="inlineStr">
@@ -28512,12 +28512,12 @@
       </c>
       <c r="C614" t="inlineStr">
         <is>
-          <t>The aggregate of nonbinary gender in a population.</t>
+          <t>A population statistic about nonbinary gender.</t>
         </is>
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>gender identity population statistic</t>
         </is>
       </c>
       <c r="E614" t="inlineStr">
@@ -28662,12 +28662,12 @@
       </c>
       <c r="C617" t="inlineStr">
         <is>
-          <t>The aggregate of not seeking employment in a population.</t>
+          <t>A population statistic about not seeking employment.</t>
         </is>
       </c>
       <c r="D617" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E617" t="inlineStr">
@@ -28812,12 +28812,12 @@
       </c>
       <c r="C620" t="inlineStr">
         <is>
-          <t>The aggregate of not working for health reasons in a population.</t>
+          <t>A population statistic about not working for health reasons.</t>
         </is>
       </c>
       <c r="D620" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E620" t="inlineStr">
@@ -28962,12 +28962,12 @@
       </c>
       <c r="C623" t="inlineStr">
         <is>
-          <t>The aggregate of number of years in education completed in a population.</t>
+          <t>A population statistic about number of years in education completed.</t>
         </is>
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>data item population statistic</t>
         </is>
       </c>
       <c r="E623" t="inlineStr">
@@ -29212,12 +29212,12 @@
       </c>
       <c r="C628" t="inlineStr">
         <is>
-          <t>The aggregate of occupational role in a population.</t>
+          <t>A population statistic about occupational role.</t>
         </is>
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal role population statistic</t>
         </is>
       </c>
       <c r="E628" t="inlineStr">
@@ -29362,12 +29362,12 @@
       </c>
       <c r="C631" t="inlineStr">
         <is>
-          <t>The aggregate of occupier of employer-provided housing in a population.</t>
+          <t>A population statistic about occupier of employer-provided housing.</t>
         </is>
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E631" t="inlineStr">
@@ -29512,12 +29512,12 @@
       </c>
       <c r="C634" t="inlineStr">
         <is>
-          <t>The aggregate of organisational role in a population.</t>
+          <t>A population statistic about organisational role.</t>
         </is>
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>role population statistic</t>
         </is>
       </c>
       <c r="E634" t="inlineStr">
@@ -29662,12 +29662,12 @@
       </c>
       <c r="C637" t="inlineStr">
         <is>
-          <t>The aggregate of other sexual orientation in a population.</t>
+          <t>A population statistic about other sexual orientation.</t>
         </is>
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sexual orientation population statistic</t>
         </is>
       </c>
       <c r="E637" t="inlineStr">
@@ -29812,12 +29812,12 @@
       </c>
       <c r="C640" t="inlineStr">
         <is>
-          <t>The aggregate of outpatient role in a population.</t>
+          <t>A population statistic about outpatient role.</t>
         </is>
       </c>
       <c r="D640" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>patient role population statistic</t>
         </is>
       </c>
       <c r="E640" t="inlineStr">
@@ -29962,12 +29962,12 @@
       </c>
       <c r="C643" t="inlineStr">
         <is>
-          <t>The aggregate of owner in a population.</t>
+          <t>A population statistic about owner.</t>
         </is>
       </c>
       <c r="D643" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>material entity population statistic</t>
         </is>
       </c>
       <c r="E643" t="inlineStr">
@@ -30112,12 +30112,12 @@
       </c>
       <c r="C646" t="inlineStr">
         <is>
-          <t>The aggregate of owner-occupier in a population.</t>
+          <t>A population statistic about owner-occupier.</t>
         </is>
       </c>
       <c r="D646" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E646" t="inlineStr">
@@ -30262,12 +30262,12 @@
       </c>
       <c r="C649" t="inlineStr">
         <is>
-          <t>The aggregate of parent in a population.</t>
+          <t>A population statistic about parent.</t>
         </is>
       </c>
       <c r="D649" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E649" t="inlineStr">
@@ -30412,12 +30412,12 @@
       </c>
       <c r="C652" t="inlineStr">
         <is>
-          <t>The aggregate of parental role in a population.</t>
+          <t>A population statistic about parental role.</t>
         </is>
       </c>
       <c r="D652" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>interpersonal role population statistic</t>
         </is>
       </c>
       <c r="E652" t="inlineStr">
@@ -30562,12 +30562,12 @@
       </c>
       <c r="C655" t="inlineStr">
         <is>
-          <t>The aggregate of past behaviour  in a population.</t>
+          <t>A population statistic about past behaviour .</t>
         </is>
       </c>
       <c r="D655" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>population statistic</t>
         </is>
       </c>
       <c r="E655" t="inlineStr">
@@ -30912,12 +30912,12 @@
       </c>
       <c r="C662" t="inlineStr">
         <is>
-          <t>The aggregate of patient role in a population.</t>
+          <t>A population statistic about patient role.</t>
         </is>
       </c>
       <c r="D662" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>role population statistic</t>
         </is>
       </c>
       <c r="E662" t="inlineStr">
@@ -31062,12 +31062,12 @@
       </c>
       <c r="C665" t="inlineStr">
         <is>
-          <t>The aggregate of personal history of behavioural lapse in a population.</t>
+          <t>A population statistic about personal history of behavioural lapse.</t>
         </is>
       </c>
       <c r="D665" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E665" t="inlineStr">
@@ -31412,12 +31412,12 @@
       </c>
       <c r="C672" t="inlineStr">
         <is>
-          <t>The aggregate of personal history of events that influence behaviour  in a population.</t>
+          <t>A population statistic about personal history of events that influence behaviour .</t>
         </is>
       </c>
       <c r="D672" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>population statistic</t>
         </is>
       </c>
       <c r="E672" t="inlineStr">
@@ -31762,12 +31762,12 @@
       </c>
       <c r="C679" t="inlineStr">
         <is>
-          <t>The aggregate of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A population statistic about personal history of intervention exposure for the same outcome.</t>
         </is>
       </c>
       <c r="D679" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E679" t="inlineStr">
@@ -32112,12 +32112,12 @@
       </c>
       <c r="C686" t="inlineStr">
         <is>
-          <t>The aggregate of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A population statistic about personal history of intervention exposure for the same outcome behaviour.</t>
         </is>
       </c>
       <c r="D686" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E686" t="inlineStr">
@@ -32462,12 +32462,12 @@
       </c>
       <c r="C693" t="inlineStr">
         <is>
-          <t>The aggregate of personal history of same intervention exposure in a population.</t>
+          <t>A population statistic about personal history of same intervention exposure.</t>
         </is>
       </c>
       <c r="D693" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E693" t="inlineStr">
@@ -32812,12 +32812,12 @@
       </c>
       <c r="C700" t="inlineStr">
         <is>
-          <t>The aggregate of personal history part of intervention exposure in a population.</t>
+          <t>A population statistic about personal history part of intervention exposure.</t>
         </is>
       </c>
       <c r="D700" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal history part population statistic</t>
         </is>
       </c>
       <c r="E700" t="inlineStr">
@@ -33162,12 +33162,12 @@
       </c>
       <c r="C707" t="inlineStr">
         <is>
-          <t>The aggregate of personal psychological attribute in a population.</t>
+          <t>A population statistic about personal psychological attribute.</t>
         </is>
       </c>
       <c r="D707" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E707" t="inlineStr">
@@ -33512,12 +33512,12 @@
       </c>
       <c r="C714" t="inlineStr">
         <is>
-          <t>The aggregate of personal vulnerability in a population.</t>
+          <t>A population statistic about personal vulnerability.</t>
         </is>
       </c>
       <c r="D714" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>disposition population statistic</t>
         </is>
       </c>
       <c r="E714" t="inlineStr">
@@ -33862,12 +33862,12 @@
       </c>
       <c r="C721" t="inlineStr">
         <is>
-          <t>The aggregate of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A population statistic about personal vulnerability to harmful behaviour.</t>
         </is>
       </c>
       <c r="D721" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal vulnerability population statistic</t>
         </is>
       </c>
       <c r="E721" t="inlineStr">
@@ -34212,12 +34212,12 @@
       </c>
       <c r="C728" t="inlineStr">
         <is>
-          <t>The aggregate of place of residence in a population.</t>
+          <t>A population statistic about place of residence.</t>
         </is>
       </c>
       <c r="D728" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>geographic location population statistic</t>
         </is>
       </c>
       <c r="E728" t="inlineStr">
@@ -34362,12 +34362,12 @@
       </c>
       <c r="C731" t="inlineStr">
         <is>
-          <t>The aggregate of policy holder role in a population.</t>
+          <t>A population statistic about policy holder role.</t>
         </is>
       </c>
       <c r="D731" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>insured party role population statistic</t>
         </is>
       </c>
       <c r="E731" t="inlineStr">
@@ -34512,12 +34512,12 @@
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>The aggregate of preschool student role in a population.</t>
+          <t>A population statistic about preschool student role.</t>
         </is>
       </c>
       <c r="D734" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>student or trainee role population statistic</t>
         </is>
       </c>
       <c r="E734" t="inlineStr">
@@ -34662,12 +34662,12 @@
       </c>
       <c r="C737" t="inlineStr">
         <is>
-          <t>The aggregate of protective factor for harmful behaviour in a population.</t>
+          <t>A population statistic about protective factor for harmful behaviour.</t>
         </is>
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>disposition population statistic</t>
         </is>
       </c>
       <c r="E737" t="inlineStr">
@@ -35012,12 +35012,12 @@
       </c>
       <c r="C744" t="inlineStr">
         <is>
-          <t>The aggregate of quantity of valuable material resource owned in a population.</t>
+          <t>A population statistic about quantity of valuable material resource owned.</t>
         </is>
       </c>
       <c r="D744" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>data item population statistic</t>
         </is>
       </c>
       <c r="E744" t="inlineStr">
@@ -35262,12 +35262,12 @@
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>The aggregate of queer in a population.</t>
+          <t>A population statistic about queer.</t>
         </is>
       </c>
       <c r="D749" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sexual orientation population statistic</t>
         </is>
       </c>
       <c r="E749" t="inlineStr">
@@ -35412,12 +35412,12 @@
       </c>
       <c r="C752" t="inlineStr">
         <is>
-          <t>The aggregate of questioning sexual orientation in a population.</t>
+          <t>A population statistic about questioning sexual orientation.</t>
         </is>
       </c>
       <c r="D752" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>self-identity population statistic</t>
         </is>
       </c>
       <c r="E752" t="inlineStr">
@@ -35562,12 +35562,12 @@
       </c>
       <c r="C755" t="inlineStr">
         <is>
-          <t>The aggregate of relationship status in a population.</t>
+          <t>A population statistic about relationship status.</t>
         </is>
       </c>
       <c r="D755" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E755" t="inlineStr">
@@ -35712,12 +35712,12 @@
       </c>
       <c r="C758" t="inlineStr">
         <is>
-          <t>The aggregate of religious group membership in a population.</t>
+          <t>A population statistic about religious group membership.</t>
         </is>
       </c>
       <c r="D758" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E758" t="inlineStr">
@@ -35862,12 +35862,12 @@
       </c>
       <c r="C761" t="inlineStr">
         <is>
-          <t>The aggregate of rent-free occupier in a population.</t>
+          <t>A population statistic about rent-free occupier.</t>
         </is>
       </c>
       <c r="D761" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E761" t="inlineStr">
@@ -36012,12 +36012,12 @@
       </c>
       <c r="C764" t="inlineStr">
         <is>
-          <t>The aggregate of rent-free occupier without owner's permission in a population.</t>
+          <t>A population statistic about rent-free occupier without owner's permission.</t>
         </is>
       </c>
       <c r="D764" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>rent-free occupier population statistic</t>
         </is>
       </c>
       <c r="E764" t="inlineStr">
@@ -36162,12 +36162,12 @@
       </c>
       <c r="C767" t="inlineStr">
         <is>
-          <t>The aggregate of renter in a population.</t>
+          <t>A population statistic about renter.</t>
         </is>
       </c>
       <c r="D767" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E767" t="inlineStr">
@@ -36312,12 +36312,12 @@
       </c>
       <c r="C770" t="inlineStr">
         <is>
-          <t>The aggregate of renter of housing from a social provider in a population.</t>
+          <t>A population statistic about renter of housing from a social provider.</t>
         </is>
       </c>
       <c r="D770" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>renter population statistic</t>
         </is>
       </c>
       <c r="E770" t="inlineStr">
@@ -36462,12 +36462,12 @@
       </c>
       <c r="C773" t="inlineStr">
         <is>
-          <t>The aggregate of residential facility owner in a population.</t>
+          <t>A population statistic about residential facility owner.</t>
         </is>
       </c>
       <c r="D773" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>owner population statistic</t>
         </is>
       </c>
       <c r="E773" t="inlineStr">
@@ -36612,12 +36612,12 @@
       </c>
       <c r="C776" t="inlineStr">
         <is>
-          <t>The aggregate of retired status in a population.</t>
+          <t>A population statistic about retired status.</t>
         </is>
       </c>
       <c r="D776" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E776" t="inlineStr">
@@ -36762,12 +36762,12 @@
       </c>
       <c r="C779" t="inlineStr">
         <is>
-          <t>The aggregate of school student role in a population.</t>
+          <t>A population statistic about school student role.</t>
         </is>
       </c>
       <c r="D779" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>student or trainee role population statistic</t>
         </is>
       </c>
       <c r="E779" t="inlineStr">
@@ -36912,12 +36912,12 @@
       </c>
       <c r="C782" t="inlineStr">
         <is>
-          <t>The aggregate of second generation immigrant in a population.</t>
+          <t>A population statistic about second generation immigrant.</t>
         </is>
       </c>
       <c r="D782" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E782" t="inlineStr">
@@ -37062,12 +37062,12 @@
       </c>
       <c r="C785" t="inlineStr">
         <is>
-          <t>The aggregate of self employed status in a population.</t>
+          <t>A population statistic about self employed status.</t>
         </is>
       </c>
       <c r="D785" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E785" t="inlineStr">
@@ -37212,12 +37212,12 @@
       </c>
       <c r="C788" t="inlineStr">
         <is>
-          <t>The aggregate of sexual orientation in a population.</t>
+          <t>A population statistic about sexual orientation.</t>
         </is>
       </c>
       <c r="D788" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E788" t="inlineStr">
@@ -37362,12 +37362,12 @@
       </c>
       <c r="C791" t="inlineStr">
         <is>
-          <t>The aggregate of sibling in a population.</t>
+          <t>A population statistic about sibling.</t>
         </is>
       </c>
       <c r="D791" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E791" t="inlineStr">
@@ -37512,12 +37512,12 @@
       </c>
       <c r="C794" t="inlineStr">
         <is>
-          <t>The aggregate of single in a population.</t>
+          <t>A population statistic about single.</t>
         </is>
       </c>
       <c r="D794" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>relationship status population statistic</t>
         </is>
       </c>
       <c r="E794" t="inlineStr">
@@ -37662,12 +37662,12 @@
       </c>
       <c r="C797" t="inlineStr">
         <is>
-          <t>The aggregate of socioeconomic status category in a population.</t>
+          <t>A population statistic about socioeconomic status category.</t>
         </is>
       </c>
       <c r="D797" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>data item population statistic</t>
         </is>
       </c>
       <c r="E797" t="inlineStr">
@@ -37812,12 +37812,12 @@
       </c>
       <c r="C800" t="inlineStr">
         <is>
-          <t>The aggregate of socioeconomic status score in a population.</t>
+          <t>A population statistic about socioeconomic status score.</t>
         </is>
       </c>
       <c r="D800" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>data item population statistic</t>
         </is>
       </c>
       <c r="E800" t="inlineStr">
@@ -38062,12 +38062,12 @@
       </c>
       <c r="C805" t="inlineStr">
         <is>
-          <t>The aggregate of stay at home parent or guardian status in a population.</t>
+          <t>A population statistic about stay at home parent or guardian status.</t>
         </is>
       </c>
       <c r="D805" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E805" t="inlineStr">
@@ -38212,12 +38212,12 @@
       </c>
       <c r="C808" t="inlineStr">
         <is>
-          <t>The aggregate of step-parent in a population.</t>
+          <t>A population statistic about step-parent.</t>
         </is>
       </c>
       <c r="D808" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>parent population statistic</t>
         </is>
       </c>
       <c r="E808" t="inlineStr">
@@ -38362,12 +38362,12 @@
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>The aggregate of step-sibling in a population.</t>
+          <t>A population statistic about step-sibling.</t>
         </is>
       </c>
       <c r="D811" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sibling population statistic</t>
         </is>
       </c>
       <c r="E811" t="inlineStr">
@@ -38512,12 +38512,12 @@
       </c>
       <c r="C814" t="inlineStr">
         <is>
-          <t>The aggregate of stepbrother in a population.</t>
+          <t>A population statistic about stepbrother.</t>
         </is>
       </c>
       <c r="D814" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>step-sibling population statistic</t>
         </is>
       </c>
       <c r="E814" t="inlineStr">
@@ -38662,12 +38662,12 @@
       </c>
       <c r="C817" t="inlineStr">
         <is>
-          <t>The aggregate of stepchild in a population.</t>
+          <t>A population statistic about stepchild.</t>
         </is>
       </c>
       <c r="D817" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>child relation population statistic</t>
         </is>
       </c>
       <c r="E817" t="inlineStr">
@@ -38812,12 +38812,12 @@
       </c>
       <c r="C820" t="inlineStr">
         <is>
-          <t>The aggregate of stepdaughter in a population.</t>
+          <t>A population statistic about stepdaughter.</t>
         </is>
       </c>
       <c r="D820" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>stepchild population statistic</t>
         </is>
       </c>
       <c r="E820" t="inlineStr">
@@ -38962,12 +38962,12 @@
       </c>
       <c r="C823" t="inlineStr">
         <is>
-          <t>The aggregate of stepfather in a population.</t>
+          <t>A population statistic about stepfather.</t>
         </is>
       </c>
       <c r="D823" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>step-parent population statistic</t>
         </is>
       </c>
       <c r="E823" t="inlineStr">
@@ -39112,12 +39112,12 @@
       </c>
       <c r="C826" t="inlineStr">
         <is>
-          <t>The aggregate of stepmother in a population.</t>
+          <t>A population statistic about stepmother.</t>
         </is>
       </c>
       <c r="D826" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>step-parent population statistic</t>
         </is>
       </c>
       <c r="E826" t="inlineStr">
@@ -39262,12 +39262,12 @@
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>The aggregate of stepsister in a population.</t>
+          <t>A population statistic about stepsister.</t>
         </is>
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>step-sibling population statistic</t>
         </is>
       </c>
       <c r="E829" t="inlineStr">
@@ -39412,12 +39412,12 @@
       </c>
       <c r="C832" t="inlineStr">
         <is>
-          <t>The aggregate of stepson in a population.</t>
+          <t>A population statistic about stepson.</t>
         </is>
       </c>
       <c r="D832" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>stepchild population statistic</t>
         </is>
       </c>
       <c r="E832" t="inlineStr">
@@ -39562,12 +39562,12 @@
       </c>
       <c r="C835" t="inlineStr">
         <is>
-          <t>The aggregate of student or trainee role in a population.</t>
+          <t>A population statistic about student or trainee role.</t>
         </is>
       </c>
       <c r="D835" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>role population statistic</t>
         </is>
       </c>
       <c r="E835" t="inlineStr">
@@ -39712,12 +39712,12 @@
       </c>
       <c r="C838" t="inlineStr">
         <is>
-          <t>The aggregate of teenager in a population.</t>
+          <t>A population statistic about teenager.</t>
         </is>
       </c>
       <c r="D838" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>person population statistic</t>
         </is>
       </c>
       <c r="E838" t="inlineStr">
@@ -39862,12 +39862,12 @@
       </c>
       <c r="C841" t="inlineStr">
         <is>
-          <t>The aggregate of transgender in a population.</t>
+          <t>A population statistic about transgender.</t>
         </is>
       </c>
       <c r="D841" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>gender identity population statistic</t>
         </is>
       </c>
       <c r="E841" t="inlineStr">
@@ -40012,12 +40012,12 @@
       </c>
       <c r="C844" t="inlineStr">
         <is>
-          <t>The aggregate of twin in a population.</t>
+          <t>A population statistic about twin.</t>
         </is>
       </c>
       <c r="D844" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>sibling population statistic</t>
         </is>
       </c>
       <c r="E844" t="inlineStr">
@@ -40162,12 +40162,12 @@
       </c>
       <c r="C847" t="inlineStr">
         <is>
-          <t>The aggregate of unawareness of a behaviour in a population.</t>
+          <t>A population statistic about unawareness of a behaviour.</t>
         </is>
       </c>
       <c r="D847" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>situational personal attribute population statistic</t>
         </is>
       </c>
       <c r="E847" t="inlineStr">
@@ -40312,12 +40312,12 @@
       </c>
       <c r="C850" t="inlineStr">
         <is>
-          <t>The aggregate of uncle in a population.</t>
+          <t>A population statistic about uncle.</t>
         </is>
       </c>
       <c r="D850" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>family member population statistic</t>
         </is>
       </c>
       <c r="E850" t="inlineStr">
@@ -40462,12 +40462,12 @@
       </c>
       <c r="C853" t="inlineStr">
         <is>
-          <t>The aggregate of undecidedness about enacting a behaviour in a population.</t>
+          <t>A population statistic about undecidedness about enacting a behaviour.</t>
         </is>
       </c>
       <c r="D853" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>situational personal attribute population statistic</t>
         </is>
       </c>
       <c r="E853" t="inlineStr">
@@ -40612,12 +40612,12 @@
       </c>
       <c r="C856" t="inlineStr">
         <is>
-          <t>The aggregate of undergraduate student role in a population.</t>
+          <t>A population statistic about undergraduate student role.</t>
         </is>
       </c>
       <c r="D856" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>higher education student role population statistic</t>
         </is>
       </c>
       <c r="E856" t="inlineStr">
@@ -40762,12 +40762,12 @@
       </c>
       <c r="C859" t="inlineStr">
         <is>
-          <t>The aggregate of unemployed in a population.</t>
+          <t>A population statistic about unemployed.</t>
         </is>
       </c>
       <c r="D859" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>employment status population statistic</t>
         </is>
       </c>
       <c r="E859" t="inlineStr">
@@ -40912,12 +40912,12 @@
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>The aggregate of unpaid carer for an adult status in a population.</t>
+          <t>A population statistic about unpaid carer for an adult status.</t>
         </is>
       </c>
       <c r="D862" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E862" t="inlineStr">
@@ -41062,12 +41062,12 @@
       </c>
       <c r="C865" t="inlineStr">
         <is>
-          <t>The aggregate of value of valuable material resource owned in a population.</t>
+          <t>A population statistic about value of valuable material resource owned.</t>
         </is>
       </c>
       <c r="D865" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>data item population statistic</t>
         </is>
       </c>
       <c r="E865" t="inlineStr">
@@ -41312,12 +41312,12 @@
       </c>
       <c r="C870" t="inlineStr">
         <is>
-          <t>The aggregate of vocational training student or trainee role in a population.</t>
+          <t>A population statistic about vocational training student or trainee role.</t>
         </is>
       </c>
       <c r="D870" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>student or trainee role population statistic</t>
         </is>
       </c>
       <c r="E870" t="inlineStr">
@@ -41462,12 +41462,12 @@
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>The aggregate of voluntary worker status in a population.</t>
+          <t>A population statistic about voluntary worker status.</t>
         </is>
       </c>
       <c r="D873" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>personal attribute population statistic</t>
         </is>
       </c>
       <c r="E873" t="inlineStr">
@@ -41612,12 +41612,12 @@
       </c>
       <c r="C876" t="inlineStr">
         <is>
-          <t>The aggregate of widowed in a population.</t>
+          <t>A population statistic about widowed.</t>
         </is>
       </c>
       <c r="D876" t="inlineStr">
         <is>
-          <t>data item</t>
+          <t>relationship status population statistic</t>
         </is>
       </c>
       <c r="E876" t="inlineStr">

</xml_diff>

<commit_message>
Fixed double spaces error in expansion script
</commit_message>
<xml_diff>
--- a/Population/BCIO_Population_Expanded.xlsx
+++ b/Population/BCIO_Population_Expanded.xlsx
@@ -9517,7 +9517,7 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>linguistic capability  population statistic</t>
+          <t>linguistic capability population statistic</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
@@ -9667,7 +9667,7 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>linguistic capability  population statistic</t>
+          <t>linguistic capability population statistic</t>
         </is>
       </c>
       <c r="E237" t="inlineStr">
@@ -9817,7 +9817,7 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>linguistic capability  population statistic</t>
+          <t>linguistic capability population statistic</t>
         </is>
       </c>
       <c r="E240" t="inlineStr">
@@ -9967,7 +9967,7 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>linguistic capability  population statistic</t>
+          <t>linguistic capability population statistic</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
@@ -25217,7 +25217,7 @@
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>linguistic capability  population statistic</t>
+          <t>linguistic capability population statistic</t>
         </is>
       </c>
       <c r="E548" t="inlineStr">

</xml_diff>

<commit_message>
Updated population expansion script to match new pattern #1087
</commit_message>
<xml_diff>
--- a/Population/BCIO_Population_Expanded.xlsx
+++ b/Population/BCIO_Population_Expanded.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -10516,7 +10516,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>The percentage of ability to comprehend spoken intervention language in a population.</t>
+          <t>A ability to comprehend spoken intervention language population statistic that is the percentage of people that have a ability to comprehend spoken intervention language in the population.</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -10567,7 +10567,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>The proportion of ability to comprehend spoken intervention language in a population.</t>
+          <t>A ability to comprehend spoken intervention language population statistic that is the proportion of people that have a ability to comprehend spoken intervention language in the population.</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -10669,7 +10669,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>The percentage of ability to read in intervention language in a population.</t>
+          <t>A ability to read in intervention language population statistic that is the percentage of people that have a ability to read in intervention language in the population.</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -10720,7 +10720,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>The proportion of ability to read in intervention language in a population.</t>
+          <t>A ability to read in intervention language population statistic that is the proportion of people that have a ability to read in intervention language in the population.</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -10822,7 +10822,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>The percentage of ability to speak in intervention language in a population.</t>
+          <t>A ability to speak in intervention language population statistic that is the percentage of people that have a ability to speak in intervention language in the population.</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -10873,7 +10873,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>The proportion of ability to speak in intervention language in a population.</t>
+          <t>A ability to speak in intervention language population statistic that is the proportion of people that have a ability to speak in intervention language in the population.</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -10975,7 +10975,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>The percentage of ability to write in intervention language in a population.</t>
+          <t>A ability to write in intervention language population statistic that is the percentage of people that have a ability to write in intervention language in the population.</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -11026,7 +11026,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>The proportion of ability to write in intervention language in a population.</t>
+          <t>A ability to write in intervention language population statistic that is the proportion of people that have a ability to write in intervention language in the population.</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -11128,7 +11128,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>The percentage of achieved bachelor's degree or equivalent level in a population.</t>
+          <t>A achieved bachelor's degree or equivalent level population statistic that is the percentage of people that have achieved bachelor's degree or equivalent level in the population.</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -11179,7 +11179,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>The proportion of achieved bachelor's degree or equivalent level in a population.</t>
+          <t>A achieved bachelor's degree or equivalent level population statistic that is the proportion of people that have achieved bachelor's degree or equivalent level in the population.</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -11281,7 +11281,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>The percentage of achieved doctoral or equivalent level education in a population.</t>
+          <t>A achieved doctoral or equivalent level education population statistic that is the percentage of people that have achieved doctoral or equivalent level education in the population.</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -11332,7 +11332,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>The proportion of achieved doctoral or equivalent level education in a population.</t>
+          <t>A achieved doctoral or equivalent level education population statistic that is the proportion of people that have achieved doctoral or equivalent level education in the population.</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -11434,7 +11434,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>The percentage of achieved early childhood education in a population.</t>
+          <t>A achieved early childhood education population statistic that is the percentage of people that have achieved early childhood education in the population.</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -11485,7 +11485,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>The proportion of achieved early childhood education in a population.</t>
+          <t>A achieved early childhood education population statistic that is the proportion of people that have achieved early childhood education in the population.</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -11587,7 +11587,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>The percentage of achieved lower secondary education in a population.</t>
+          <t>A achieved lower secondary education population statistic that is the percentage of people that have achieved lower secondary education in the population.</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -11638,7 +11638,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>The proportion of achieved lower secondary education in a population.</t>
+          <t>A achieved lower secondary education population statistic that is the proportion of people that have achieved lower secondary education in the population.</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -11740,7 +11740,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>The percentage of achieved master's or equivalent level in a population.</t>
+          <t>A achieved master's or equivalent level population statistic that is the percentage of people that have achieved master's or equivalent level in the population.</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -11791,7 +11791,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>The proportion of achieved master's or equivalent level in a population.</t>
+          <t>A achieved master's or equivalent level population statistic that is the proportion of people that have achieved master's or equivalent level in the population.</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -11893,7 +11893,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>The percentage of achieved primary education in a population.</t>
+          <t>A achieved primary education population statistic that is the percentage of people that have achieved primary education in the population.</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -11944,7 +11944,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>The proportion of achieved primary education in a population.</t>
+          <t>A achieved primary education population statistic that is the proportion of people that have achieved primary education in the population.</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -12046,7 +12046,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>The percentage of achieved upper secondary education  in a population.</t>
+          <t>A achieved upper secondary education  population statistic that is the percentage of people that have achieved upper secondary education  in the population.</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
@@ -12097,7 +12097,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>The proportion of achieved upper secondary education  in a population.</t>
+          <t>A achieved upper secondary education  population statistic that is the proportion of people that have achieved upper secondary education  in the population.</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -12199,7 +12199,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>The percentage of adoptive brother in a population.</t>
+          <t>A adoptive brother population statistic that is the percentage of people that are a adoptive brother in the population.</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -12250,7 +12250,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>The proportion of adoptive brother in a population.</t>
+          <t>A adoptive brother population statistic that is the proportion of people that are a adoptive brother in the population.</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
@@ -12352,7 +12352,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>The percentage of adoptive child in a population.</t>
+          <t>A adoptive child population statistic that is the percentage of people that are a adoptive child in the population.</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -12403,7 +12403,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>The proportion of adoptive child in a population.</t>
+          <t>A adoptive child population statistic that is the proportion of people that are a adoptive child in the population.</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -12505,7 +12505,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>The percentage of adoptive daughter in a population.</t>
+          <t>A adoptive daughter population statistic that is the percentage of people that are a adoptive daughter in the population.</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -12556,7 +12556,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>The proportion of adoptive daughter in a population.</t>
+          <t>A adoptive daughter population statistic that is the proportion of people that are a adoptive daughter in the population.</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -12658,7 +12658,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>The percentage of adoptive father in a population.</t>
+          <t>A adoptive father population statistic that is the percentage of people that are a adoptive father in the population.</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -12709,7 +12709,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>The proportion of adoptive father in a population.</t>
+          <t>A adoptive father population statistic that is the proportion of people that are a adoptive father in the population.</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -12811,7 +12811,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>The percentage of adoptive mother in a population.</t>
+          <t>A adoptive mother population statistic that is the percentage of people that are a adoptive mother in the population.</t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
@@ -12862,7 +12862,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>The proportion of adoptive mother in a population.</t>
+          <t>A adoptive mother population statistic that is the proportion of people that are a adoptive mother in the population.</t>
         </is>
       </c>
       <c r="D281" t="inlineStr">
@@ -12964,7 +12964,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>The percentage of adoptive parent in a population.</t>
+          <t>A adoptive parent population statistic that is the percentage of people that are a adoptive parent in the population.</t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
@@ -13015,7 +13015,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>The proportion of adoptive parent in a population.</t>
+          <t>A adoptive parent population statistic that is the proportion of people that are a adoptive parent in the population.</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -13117,7 +13117,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>The percentage of adoptive sibling in a population.</t>
+          <t>A adoptive sibling population statistic that is the percentage of people that are a adoptive sibling in the population.</t>
         </is>
       </c>
       <c r="D286" t="inlineStr">
@@ -13168,7 +13168,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>The proportion of adoptive sibling in a population.</t>
+          <t>A adoptive sibling population statistic that is the proportion of people that are a adoptive sibling in the population.</t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
@@ -13270,7 +13270,7 @@
       </c>
       <c r="C289" t="inlineStr">
         <is>
-          <t>The percentage of adoptive sister in a population.</t>
+          <t>A adoptive sister population statistic that is the percentage of people that are a adoptive sister in the population.</t>
         </is>
       </c>
       <c r="D289" t="inlineStr">
@@ -13321,7 +13321,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>The proportion of adoptive sister in a population.</t>
+          <t>A adoptive sister population statistic that is the proportion of people that are a adoptive sister in the population.</t>
         </is>
       </c>
       <c r="D290" t="inlineStr">
@@ -13423,7 +13423,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>The percentage of adoptive son in a population.</t>
+          <t>A adoptive son population statistic that is the percentage of people that are a adoptive son in the population.</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -13474,7 +13474,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>The proportion of adoptive son in a population.</t>
+          <t>A adoptive son population statistic that is the proportion of people that are a adoptive son in the population.</t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
@@ -13576,7 +13576,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>The percentage of adult in a population.</t>
+          <t>A adult population statistic that is the percentage of people that are a adult in the population.</t>
         </is>
       </c>
       <c r="D295" t="inlineStr">
@@ -13627,7 +13627,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>The proportion of adult in a population.</t>
+          <t>A adult population statistic that is the proportion of people that are a adult in the population.</t>
         </is>
       </c>
       <c r="D296" t="inlineStr">
@@ -13729,7 +13729,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>The percentage of agreed rent-free occupier in a population.</t>
+          <t>A agreed rent-free occupier population statistic that is the percentage of people that are a agreed rent-free occupier in the population.</t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
@@ -13780,7 +13780,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>The proportion of agreed rent-free occupier in a population.</t>
+          <t>A agreed rent-free occupier population statistic that is the proportion of people that are a agreed rent-free occupier in the population.</t>
         </is>
       </c>
       <c r="D299" t="inlineStr">
@@ -13882,7 +13882,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>The percentage of asexual in a population.</t>
+          <t>A asexual population statistic that is the percentage of people that are asexual in the population.</t>
         </is>
       </c>
       <c r="D301" t="inlineStr">
@@ -13933,7 +13933,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>The proportion of asexual in a population.</t>
+          <t>A asexual population statistic that is the proportion of people that are asexual in the population.</t>
         </is>
       </c>
       <c r="D302" t="inlineStr">
@@ -14035,7 +14035,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>The percentage of aunt in a population.</t>
+          <t>A aunt population statistic that is the percentage of people that are a aunt in the population.</t>
         </is>
       </c>
       <c r="D304" t="inlineStr">
@@ -14086,7 +14086,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>The proportion of aunt in a population.</t>
+          <t>A aunt population statistic that is the proportion of people that are a aunt in the population.</t>
         </is>
       </c>
       <c r="D305" t="inlineStr">
@@ -14188,7 +14188,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>The percentage of biological brother in a population.</t>
+          <t>A biological brother population statistic that is the percentage of people that are a biological brother in the population.</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
@@ -14239,7 +14239,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>The proportion of biological brother in a population.</t>
+          <t>A biological brother population statistic that is the proportion of people that are a biological brother in the population.</t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
@@ -14341,7 +14341,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>The percentage of biological child in a population.</t>
+          <t>A biological child population statistic that is the percentage of people that are a biological child in the population.</t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
@@ -14392,7 +14392,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>The proportion of biological child in a population.</t>
+          <t>A biological child population statistic that is the proportion of people that are a biological child in the population.</t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
@@ -14494,7 +14494,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>The percentage of biological daughter in a population.</t>
+          <t>A biological daughter population statistic that is the percentage of people that are a biological daughter in the population.</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -14545,7 +14545,7 @@
       </c>
       <c r="C314" t="inlineStr">
         <is>
-          <t>The proportion of biological daughter in a population.</t>
+          <t>A biological daughter population statistic that is the proportion of people that are a biological daughter in the population.</t>
         </is>
       </c>
       <c r="D314" t="inlineStr">
@@ -14647,7 +14647,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>The percentage of biological father in a population.</t>
+          <t>A biological father population statistic that is the percentage of people that are a biological father in the population.</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
@@ -14698,7 +14698,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>The proportion of biological father in a population.</t>
+          <t>A biological father population statistic that is the proportion of people that are a biological father in the population.</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
@@ -14800,7 +14800,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>The percentage of biological mother in a population.</t>
+          <t>A biological mother population statistic that is the percentage of people that are a biological mother in the population.</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
@@ -14851,7 +14851,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>The proportion of biological mother in a population.</t>
+          <t>A biological mother population statistic that is the proportion of people that are a biological mother in the population.</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
@@ -14953,7 +14953,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>The percentage of biological parent in a population.</t>
+          <t>A biological parent population statistic that is the percentage of people that are a biological parent in the population.</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
@@ -15004,7 +15004,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>The proportion of biological parent in a population.</t>
+          <t>A biological parent population statistic that is the proportion of people that are a biological parent in the population.</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
@@ -15106,7 +15106,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>The percentage of biological sex in a population.</t>
+          <t>A biological sex population statistic that is the percentage of people that have a biological sex in the population.</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
@@ -15157,7 +15157,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>The proportion of biological sex in a population.</t>
+          <t>A biological sex population statistic that is the proportion of people that have a biological sex in the population.</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
@@ -15259,7 +15259,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>The percentage of biological sibling in a population.</t>
+          <t>A biological sibling population statistic that is the percentage of people that are a biological sibling in the population.</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
@@ -15310,7 +15310,7 @@
       </c>
       <c r="C329" t="inlineStr">
         <is>
-          <t>The proportion of biological sibling in a population.</t>
+          <t>A biological sibling population statistic that is the proportion of people that are a biological sibling in the population.</t>
         </is>
       </c>
       <c r="D329" t="inlineStr">
@@ -15412,7 +15412,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>The percentage of biological sister in a population.</t>
+          <t>A biological sister population statistic that is the percentage of people that are a biological sister in the population.</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
@@ -15463,7 +15463,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>The proportion of biological sister in a population.</t>
+          <t>A biological sister population statistic that is the proportion of people that are a biological sister in the population.</t>
         </is>
       </c>
       <c r="D332" t="inlineStr">
@@ -15565,7 +15565,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>The percentage of biological son in a population.</t>
+          <t>A biological son population statistic that is the percentage of people that are a biological son in the population.</t>
         </is>
       </c>
       <c r="D334" t="inlineStr">
@@ -15616,7 +15616,7 @@
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>The proportion of biological son in a population.</t>
+          <t>A biological son population statistic that is the proportion of people that are a biological son in the population.</t>
         </is>
       </c>
       <c r="D335" t="inlineStr">
@@ -15718,7 +15718,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>The percentage of bisexual in a population.</t>
+          <t>A bisexual population statistic that is the percentage of people that are bisexual in the population.</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
@@ -15769,7 +15769,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>The proportion of bisexual in a population.</t>
+          <t>A bisexual population statistic that is the proportion of people that are bisexual in the population.</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
@@ -15871,7 +15871,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>The percentage of caregiving role in a population.</t>
+          <t>A caregiving role population statistic that is the percentage of people that have a caregiving role in the population.</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
@@ -15922,7 +15922,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>The proportion of caregiving role in a population.</t>
+          <t>A caregiving role population statistic that is the proportion of people that have a caregiving role in the population.</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
@@ -16024,7 +16024,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>The percentage of caste membership in a population.</t>
+          <t>A caste membership population statistic that is the percentage of people that have a caste membership in the population.</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
@@ -16075,7 +16075,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>The proportion of caste membership in a population.</t>
+          <t>A caste membership population statistic that is the proportion of people that have a caste membership in the population.</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
@@ -16177,7 +16177,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>The percentage of child in a population.</t>
+          <t>A child population statistic that is the percentage of people that are a child in the population.</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
@@ -16228,7 +16228,7 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>The proportion of child in a population.</t>
+          <t>A child population statistic that is the proportion of people that are a child in the population.</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
@@ -16330,7 +16330,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>The percentage of child relation in a population.</t>
+          <t>A child relation population statistic that is the percentage of people that have a child relation in the population.</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
@@ -16381,7 +16381,7 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>The proportion of child relation in a population.</t>
+          <t>A child relation population statistic that is the proportion of people that have a child relation in the population.</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
@@ -16483,7 +16483,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>The percentage of cisgender in a population.</t>
+          <t>A cisgender population statistic that is the percentage of people that are cisgender in the population.</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
@@ -16534,7 +16534,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>The proportion of cisgender in a population.</t>
+          <t>A cisgender population statistic that is the proportion of people that are cisgender in the population.</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
@@ -16636,7 +16636,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>The percentage of country of birth in a population.</t>
+          <t>A country of birth population statistic that is the percentage of people that have a country of birth in the population.</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
@@ -16687,7 +16687,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>The proportion of country of birth in a population.</t>
+          <t>A country of birth population statistic that is the proportion of people that have a country of birth in the population.</t>
         </is>
       </c>
       <c r="D356" t="inlineStr">
@@ -16789,7 +16789,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>The percentage of cousin in a population.</t>
+          <t>A cousin population statistic that is the percentage of people that are a cousin in the population.</t>
         </is>
       </c>
       <c r="D358" t="inlineStr">
@@ -16840,7 +16840,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>The proportion of cousin in a population.</t>
+          <t>A cousin population statistic that is the proportion of people that are a cousin in the population.</t>
         </is>
       </c>
       <c r="D359" t="inlineStr">
@@ -16942,7 +16942,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>The percentage of disabled in a population.</t>
+          <t>A disabled population statistic that is the percentage of people that are disabled in the population.</t>
         </is>
       </c>
       <c r="D361" t="inlineStr">
@@ -16993,7 +16993,7 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>The proportion of disabled in a population.</t>
+          <t>A disabled population statistic that is the proportion of people that are disabled in the population.</t>
         </is>
       </c>
       <c r="D362" t="inlineStr">
@@ -17095,7 +17095,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>The percentage of discipline of current programme of study or training in a population.</t>
+          <t>A discipline of current programme of study or training population statistic that is the percentage of people that have a discipline of current programme of study or training in the population.</t>
         </is>
       </c>
       <c r="D364" t="inlineStr">
@@ -17146,7 +17146,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>The proportion of discipline of current programme of study or training in a population.</t>
+          <t>A discipline of current programme of study or training population statistic that is the proportion of people that have a discipline of current programme of study or training in the population.</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
@@ -17248,7 +17248,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>The percentage of discipline of highest level of formal educational qualification achieved in a population.</t>
+          <t>A discipline of highest level of formal educational qualification achieved population statistic that is the percentage of people that have a discipline of highest level of formal educational qualification achieved in the population.</t>
         </is>
       </c>
       <c r="D367" t="inlineStr">
@@ -17299,7 +17299,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>The proportion of discipline of highest level of formal educational qualification achieved in a population.</t>
+          <t>A discipline of highest level of formal educational qualification achieved population statistic that is the proportion of people that have a discipline of highest level of formal educational qualification achieved in the population.</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
@@ -17401,7 +17401,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>The percentage of divorced or separated in a population.</t>
+          <t>A divorced or separated population statistic that is the percentage of people that are divorced or separated in the population.</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
@@ -17452,7 +17452,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>The proportion of divorced or separated in a population.</t>
+          <t>A divorced or separated population statistic that is the proportion of people that are divorced or separated in the population.</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
@@ -17554,7 +17554,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>The percentage of doctoral student role in a population.</t>
+          <t>A doctoral student role population statistic that is the percentage of people that are a doctoral student role in the population.</t>
         </is>
       </c>
       <c r="D373" t="inlineStr">
@@ -17605,7 +17605,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>The proportion of doctoral student role in a population.</t>
+          <t>A doctoral student role population statistic that is the proportion of people that are a doctoral student role in the population.</t>
         </is>
       </c>
       <c r="D374" t="inlineStr">
@@ -17707,7 +17707,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>The percentage of employed in a population.</t>
+          <t>A employed population statistic that is the percentage of people that are employed in the population.</t>
         </is>
       </c>
       <c r="D376" t="inlineStr">
@@ -17758,7 +17758,7 @@
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>The proportion of employed in a population.</t>
+          <t>A employed population statistic that is the proportion of people that are employed in the population.</t>
         </is>
       </c>
       <c r="D377" t="inlineStr">
@@ -17860,7 +17860,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>The percentage of employed full time in a population.</t>
+          <t>A employed full time population statistic that is the percentage of people that are employed full time in the population.</t>
         </is>
       </c>
       <c r="D379" t="inlineStr">
@@ -17911,7 +17911,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>The proportion of employed full time in a population.</t>
+          <t>A employed full time population statistic that is the proportion of people that are employed full time in the population.</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
@@ -18013,7 +18013,7 @@
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>The percentage of employed in shift work in a population.</t>
+          <t>A employed in shift work population statistic that is the percentage of people that are employed in shift work in the population.</t>
         </is>
       </c>
       <c r="D382" t="inlineStr">
@@ -18064,7 +18064,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>The proportion of employed in shift work in a population.</t>
+          <t>A employed in shift work population statistic that is the proportion of people that are employed in shift work in the population.</t>
         </is>
       </c>
       <c r="D383" t="inlineStr">
@@ -18166,7 +18166,7 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>The percentage of employed part time in a population.</t>
+          <t>A employed part time population statistic that is the percentage of people that are employed part time in the population.</t>
         </is>
       </c>
       <c r="D385" t="inlineStr">
@@ -18217,7 +18217,7 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>The proportion of employed part time in a population.</t>
+          <t>A employed part time population statistic that is the proportion of people that are employed part time in the population.</t>
         </is>
       </c>
       <c r="D386" t="inlineStr">
@@ -18319,7 +18319,7 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>The percentage of employment status in a population.</t>
+          <t>A employment status population statistic that is the percentage of people that have a employment status in the population.</t>
         </is>
       </c>
       <c r="D388" t="inlineStr">
@@ -18370,7 +18370,7 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>The proportion of employment status in a population.</t>
+          <t>A employment status population statistic that is the proportion of people that have a employment status in the population.</t>
         </is>
       </c>
       <c r="D389" t="inlineStr">
@@ -18472,7 +18472,7 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>The percentage of ethnic group membership in a population.</t>
+          <t>A ethnic group membership population statistic that is the percentage of people that have a ethnic group membership in the population.</t>
         </is>
       </c>
       <c r="D391" t="inlineStr">
@@ -18523,7 +18523,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>The proportion of ethnic group membership in a population.</t>
+          <t>A ethnic group membership population statistic that is the proportion of people that have a ethnic group membership in the population.</t>
         </is>
       </c>
       <c r="D392" t="inlineStr">
@@ -18625,7 +18625,7 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>The percentage of expertise discipline in a population.</t>
+          <t>A expertise discipline population statistic that is the percentage of people that have a expertise discipline in the population.</t>
         </is>
       </c>
       <c r="D394" t="inlineStr">
@@ -18676,7 +18676,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>The proportion of expertise discipline in a population.</t>
+          <t>A expertise discipline population statistic that is the proportion of people that have a expertise discipline in the population.</t>
         </is>
       </c>
       <c r="D395" t="inlineStr">
@@ -18778,7 +18778,7 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>The percentage of family member in a population.</t>
+          <t>A family member population statistic that is the percentage of people that are a family member in the population.</t>
         </is>
       </c>
       <c r="D397" t="inlineStr">
@@ -18829,7 +18829,7 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>The proportion of family member in a population.</t>
+          <t>A family member population statistic that is the proportion of people that are a family member in the population.</t>
         </is>
       </c>
       <c r="D398" t="inlineStr">
@@ -18931,7 +18931,7 @@
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>The percentage of father in a population.</t>
+          <t>A father population statistic that is the percentage of people that are a father in the population.</t>
         </is>
       </c>
       <c r="D400" t="inlineStr">
@@ -18982,7 +18982,7 @@
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>The proportion of father in a population.</t>
+          <t>A father population statistic that is the proportion of people that are a father in the population.</t>
         </is>
       </c>
       <c r="D401" t="inlineStr">
@@ -19084,7 +19084,7 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>The percentage of female biological sex in a population.</t>
+          <t>A female biological sex population statistic that is the percentage of people that have a female biological sex in the population.</t>
         </is>
       </c>
       <c r="D403" t="inlineStr">
@@ -19135,7 +19135,7 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>The proportion of female biological sex in a population.</t>
+          <t>A female biological sex population statistic that is the proportion of people that have a female biological sex in the population.</t>
         </is>
       </c>
       <c r="D404" t="inlineStr">
@@ -19237,7 +19237,7 @@
       </c>
       <c r="C406" t="inlineStr">
         <is>
-          <t>The percentage of female gender in a population.</t>
+          <t>A female gender population statistic that is the percentage of people that have a female gender in the population.</t>
         </is>
       </c>
       <c r="D406" t="inlineStr">
@@ -19288,7 +19288,7 @@
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>The proportion of female gender in a population.</t>
+          <t>A female gender population statistic that is the proportion of people that have a female gender in the population.</t>
         </is>
       </c>
       <c r="D407" t="inlineStr">
@@ -19390,7 +19390,7 @@
       </c>
       <c r="C409" t="inlineStr">
         <is>
-          <t>The percentage of foster brother in a population.</t>
+          <t>A foster brother population statistic that is the percentage of people that are a foster brother in the population.</t>
         </is>
       </c>
       <c r="D409" t="inlineStr">
@@ -19441,7 +19441,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>The proportion of foster brother in a population.</t>
+          <t>A foster brother population statistic that is the proportion of people that are a foster brother in the population.</t>
         </is>
       </c>
       <c r="D410" t="inlineStr">
@@ -19543,7 +19543,7 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>The percentage of foster child in a population.</t>
+          <t>A foster child population statistic that is the percentage of people that are a foster child in the population.</t>
         </is>
       </c>
       <c r="D412" t="inlineStr">
@@ -19594,7 +19594,7 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>The proportion of foster child in a population.</t>
+          <t>A foster child population statistic that is the proportion of people that are a foster child in the population.</t>
         </is>
       </c>
       <c r="D413" t="inlineStr">
@@ -19696,7 +19696,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>The percentage of foster daughter in a population.</t>
+          <t>A foster daughter population statistic that is the percentage of people that are a foster daughter in the population.</t>
         </is>
       </c>
       <c r="D415" t="inlineStr">
@@ -19747,7 +19747,7 @@
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>The proportion of foster daughter in a population.</t>
+          <t>A foster daughter population statistic that is the proportion of people that are a foster daughter in the population.</t>
         </is>
       </c>
       <c r="D416" t="inlineStr">
@@ -19849,7 +19849,7 @@
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>The percentage of foster father in a population.</t>
+          <t>A foster father population statistic that is the percentage of people that are a foster father in the population.</t>
         </is>
       </c>
       <c r="D418" t="inlineStr">
@@ -19900,7 +19900,7 @@
       </c>
       <c r="C419" t="inlineStr">
         <is>
-          <t>The proportion of foster father in a population.</t>
+          <t>A foster father population statistic that is the proportion of people that are a foster father in the population.</t>
         </is>
       </c>
       <c r="D419" t="inlineStr">
@@ -20002,7 +20002,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>The percentage of foster mother in a population.</t>
+          <t>A foster mother population statistic that is the percentage of people that are a foster mother in the population.</t>
         </is>
       </c>
       <c r="D421" t="inlineStr">
@@ -20053,7 +20053,7 @@
       </c>
       <c r="C422" t="inlineStr">
         <is>
-          <t>The proportion of foster mother in a population.</t>
+          <t>A foster mother population statistic that is the proportion of people that are a foster mother in the population.</t>
         </is>
       </c>
       <c r="D422" t="inlineStr">
@@ -20155,7 +20155,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>The percentage of foster parent in a population.</t>
+          <t>A foster parent population statistic that is the percentage of people that are a foster parent in the population.</t>
         </is>
       </c>
       <c r="D424" t="inlineStr">
@@ -20206,7 +20206,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>The proportion of foster parent in a population.</t>
+          <t>A foster parent population statistic that is the proportion of people that are a foster parent in the population.</t>
         </is>
       </c>
       <c r="D425" t="inlineStr">
@@ -20308,7 +20308,7 @@
       </c>
       <c r="C427" t="inlineStr">
         <is>
-          <t>The percentage of foster sibling in a population.</t>
+          <t>A foster sibling population statistic that is the percentage of people that are a foster sibling in the population.</t>
         </is>
       </c>
       <c r="D427" t="inlineStr">
@@ -20359,7 +20359,7 @@
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>The proportion of foster sibling in a population.</t>
+          <t>A foster sibling population statistic that is the proportion of people that are a foster sibling in the population.</t>
         </is>
       </c>
       <c r="D428" t="inlineStr">
@@ -20461,7 +20461,7 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>The percentage of foster sister in a population.</t>
+          <t>A foster sister population statistic that is the percentage of people that are a foster sister in the population.</t>
         </is>
       </c>
       <c r="D430" t="inlineStr">
@@ -20512,7 +20512,7 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>The proportion of foster sister in a population.</t>
+          <t>A foster sister population statistic that is the proportion of people that are a foster sister in the population.</t>
         </is>
       </c>
       <c r="D431" t="inlineStr">
@@ -20614,7 +20614,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>The percentage of foster son in a population.</t>
+          <t>A foster son population statistic that is the percentage of people that are a foster son in the population.</t>
         </is>
       </c>
       <c r="D433" t="inlineStr">
@@ -20665,7 +20665,7 @@
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>The proportion of foster son in a population.</t>
+          <t>A foster son population statistic that is the proportion of people that are a foster son in the population.</t>
         </is>
       </c>
       <c r="D434" t="inlineStr">
@@ -20767,7 +20767,7 @@
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>The percentage of gender identity in a population.</t>
+          <t>A gender identity population statistic that is the percentage of people that have a gender identity in the population.</t>
         </is>
       </c>
       <c r="D436" t="inlineStr">
@@ -20818,7 +20818,7 @@
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>The proportion of gender identity in a population.</t>
+          <t>A gender identity population statistic that is the proportion of people that have a gender identity in the population.</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
@@ -20920,7 +20920,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>The percentage of graduate student role in a population.</t>
+          <t>A graduate student role population statistic that is the percentage of people that have a graduate student role in the population.</t>
         </is>
       </c>
       <c r="D439" t="inlineStr">
@@ -20971,7 +20971,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>The proportion of graduate student role in a population.</t>
+          <t>A graduate student role population statistic that is the proportion of people that have a graduate student role in the population.</t>
         </is>
       </c>
       <c r="D440" t="inlineStr">
@@ -21073,7 +21073,7 @@
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>The percentage of grandfather in a population.</t>
+          <t>A grandfather population statistic that is the percentage of people that are a grandfather in the population.</t>
         </is>
       </c>
       <c r="D442" t="inlineStr">
@@ -21124,7 +21124,7 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>The proportion of grandfather in a population.</t>
+          <t>A grandfather population statistic that is the proportion of people that are a grandfather in the population.</t>
         </is>
       </c>
       <c r="D443" t="inlineStr">
@@ -21226,7 +21226,7 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>The percentage of grandmother in a population.</t>
+          <t>A grandmother population statistic that is the percentage of people that are a grandmother in the population.</t>
         </is>
       </c>
       <c r="D445" t="inlineStr">
@@ -21277,7 +21277,7 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>The proportion of grandmother in a population.</t>
+          <t>A grandmother population statistic that is the proportion of people that are a grandmother in the population.</t>
         </is>
       </c>
       <c r="D446" t="inlineStr">
@@ -21379,7 +21379,7 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>The percentage of grandparent in a population.</t>
+          <t>A grandparent population statistic that is the percentage of people that are a grandparent in the population.</t>
         </is>
       </c>
       <c r="D448" t="inlineStr">
@@ -21430,7 +21430,7 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>The proportion of grandparent in a population.</t>
+          <t>A grandparent population statistic that is the proportion of people that are a grandparent in the population.</t>
         </is>
       </c>
       <c r="D449" t="inlineStr">
@@ -21532,7 +21532,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>The percentage of having enacted a behaviour in a population.</t>
+          <t>A having enacted a behaviour population statistic that is the percentage of people that have having enacted a behaviour in the population.</t>
         </is>
       </c>
       <c r="D451" t="inlineStr">
@@ -21583,7 +21583,7 @@
       </c>
       <c r="C452" t="inlineStr">
         <is>
-          <t>The proportion of having enacted a behaviour in a population.</t>
+          <t>A having enacted a behaviour population statistic that is the proportion of people that have having enacted a behaviour in the population.</t>
         </is>
       </c>
       <c r="D452" t="inlineStr">
@@ -21685,7 +21685,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>The percentage of health insurance policy holder role in a population.</t>
+          <t>A health insurance policy holder role population statistic that is the percentage of people that have a health insurance policy holder role in the population.</t>
         </is>
       </c>
       <c r="D454" t="inlineStr">
@@ -21736,7 +21736,7 @@
       </c>
       <c r="C455" t="inlineStr">
         <is>
-          <t>The proportion of health insurance policy holder role in a population.</t>
+          <t>A health insurance policy holder role population statistic that is the proportion of people that have a health insurance policy holder role in the population.</t>
         </is>
       </c>
       <c r="D455" t="inlineStr">
@@ -21838,7 +21838,7 @@
       </c>
       <c r="C457" t="inlineStr">
         <is>
-          <t>The percentage of health status attribute in a population.</t>
+          <t>A health status attribute population statistic that is the percentage of people that have a health status attribute in the population.</t>
         </is>
       </c>
       <c r="D457" t="inlineStr">
@@ -21889,7 +21889,7 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>The proportion of health status attribute in a population.</t>
+          <t>A health status attribute population statistic that is the proportion of people that have a health status attribute in the population.</t>
         </is>
       </c>
       <c r="D458" t="inlineStr">
@@ -21991,7 +21991,7 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>The percentage of heterosexual in a population.</t>
+          <t>A heterosexual population statistic that is the percentage of people that are heterosexual in the population.</t>
         </is>
       </c>
       <c r="D460" t="inlineStr">
@@ -22042,7 +22042,7 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>The proportion of heterosexual in a population.</t>
+          <t>A heterosexual population statistic that is the proportion of people that are heterosexual in the population.</t>
         </is>
       </c>
       <c r="D461" t="inlineStr">
@@ -22144,7 +22144,7 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>The percentage of higher education student role in a population.</t>
+          <t>A higher education student role population statistic that is the percentage of people that have a higher education student role in the population.</t>
         </is>
       </c>
       <c r="D463" t="inlineStr">
@@ -22195,7 +22195,7 @@
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>The proportion of higher education student role in a population.</t>
+          <t>A higher education student role population statistic that is the proportion of people that have a higher education student role in the population.</t>
         </is>
       </c>
       <c r="D464" t="inlineStr">
@@ -22297,7 +22297,7 @@
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>The percentage of highest level of formal educational qualification achieved in a population.</t>
+          <t>A highest level of formal educational qualification achieved population statistic that is the percentage of people that have a highest level of formal educational qualification achieved in the population.</t>
         </is>
       </c>
       <c r="D466" t="inlineStr">
@@ -22348,7 +22348,7 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>The proportion of highest level of formal educational qualification achieved in a population.</t>
+          <t>A highest level of formal educational qualification achieved population statistic that is the proportion of people that have a highest level of formal educational qualification achieved in the population.</t>
         </is>
       </c>
       <c r="D467" t="inlineStr">
@@ -22450,7 +22450,7 @@
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>The percentage of history of exposure to an occupational hazard in a population.</t>
+          <t>A history of exposure to an occupational hazard population statistic that is the percentage of people that have a history of exposure to an occupational hazard in the population.</t>
         </is>
       </c>
       <c r="D469" t="inlineStr">
@@ -22501,7 +22501,7 @@
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>The proportion of history of exposure to an occupational hazard in a population.</t>
+          <t>A history of exposure to an occupational hazard population statistic that is the proportion of people that have a history of exposure to an occupational hazard in the population.</t>
         </is>
       </c>
       <c r="D470" t="inlineStr">
@@ -22603,7 +22603,7 @@
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>The percentage of history of exposure to childhood maltreatment in a population.</t>
+          <t>A history of exposure to childhood maltreatment population statistic that is the percentage of people that have a history of exposure to childhood maltreatment in the population.</t>
         </is>
       </c>
       <c r="D472" t="inlineStr">
@@ -22654,7 +22654,7 @@
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>The proportion of history of exposure to childhood maltreatment in a population.</t>
+          <t>A history of exposure to childhood maltreatment population statistic that is the proportion of people that have a history of exposure to childhood maltreatment in the population.</t>
         </is>
       </c>
       <c r="D473" t="inlineStr">
@@ -22756,7 +22756,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>The percentage of homeless person in a population.</t>
+          <t>A homeless person population statistic that is the percentage of people that are a homeless person in the population.</t>
         </is>
       </c>
       <c r="D475" t="inlineStr">
@@ -22807,7 +22807,7 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>The proportion of homeless person in a population.</t>
+          <t>A homeless person population statistic that is the proportion of people that are a homeless person in the population.</t>
         </is>
       </c>
       <c r="D476" t="inlineStr">
@@ -22909,7 +22909,7 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>The percentage of homemaker status in a population.</t>
+          <t>A homemaker status population statistic that is the percentage of people that have a homemaker status in the population.</t>
         </is>
       </c>
       <c r="D478" t="inlineStr">
@@ -22960,7 +22960,7 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>The proportion of homemaker status in a population.</t>
+          <t>A homemaker status population statistic that is the proportion of people that have a homemaker status in the population.</t>
         </is>
       </c>
       <c r="D479" t="inlineStr">
@@ -23062,7 +23062,7 @@
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>The percentage of homosexual in a population.</t>
+          <t>A homosexual population statistic that is the percentage of people that are homosexual in the population.</t>
         </is>
       </c>
       <c r="D481" t="inlineStr">
@@ -23113,7 +23113,7 @@
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>The proportion of homosexual in a population.</t>
+          <t>A homosexual population statistic that is the proportion of people that are homosexual in the population.</t>
         </is>
       </c>
       <c r="D482" t="inlineStr">
@@ -23215,7 +23215,7 @@
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>The mean of household income in a population.</t>
+          <t>A household income population statistic that is the mean value of household income in the population.</t>
         </is>
       </c>
       <c r="D484" t="inlineStr">
@@ -23266,7 +23266,7 @@
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>The minimum of household income in a population.</t>
+          <t>A household income population statistic that is the minimum value of household income in the population.</t>
         </is>
       </c>
       <c r="D485" t="inlineStr">
@@ -23317,7 +23317,7 @@
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>The maximum of household income in a population.</t>
+          <t>A household income population statistic that is the maximum value of household income in the population.</t>
         </is>
       </c>
       <c r="D486" t="inlineStr">
@@ -23368,7 +23368,7 @@
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>The median of household income in a population.</t>
+          <t>A household income population statistic that is the median value of household income in the population.</t>
         </is>
       </c>
       <c r="D487" t="inlineStr">
@@ -23419,7 +23419,7 @@
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>The percentage of household income in a population.</t>
+          <t>A household income population statistic that is the percentage value of household income in the population.</t>
         </is>
       </c>
       <c r="D488" t="inlineStr">
@@ -23470,7 +23470,7 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>The proportion of household income in a population.</t>
+          <t>A household income population statistic that is the proportion of individuals having a household income in the population.</t>
         </is>
       </c>
       <c r="D489" t="inlineStr">
@@ -23572,7 +23572,7 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>The mean of human age in a population.</t>
+          <t>A human age population statistic that is the mean value of human age in the population.</t>
         </is>
       </c>
       <c r="D491" t="inlineStr">
@@ -23623,7 +23623,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>The minimum of human age in a population.</t>
+          <t>A human age population statistic that is the minimum value of human age in the population.</t>
         </is>
       </c>
       <c r="D492" t="inlineStr">
@@ -23674,7 +23674,7 @@
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>The maximum of human age in a population.</t>
+          <t>A human age population statistic that is the maximum value of human age in the population.</t>
         </is>
       </c>
       <c r="D493" t="inlineStr">
@@ -23725,7 +23725,7 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>The median of human age in a population.</t>
+          <t>A human age population statistic that is the median value of human age in the population.</t>
         </is>
       </c>
       <c r="D494" t="inlineStr">
@@ -23827,7 +23827,7 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>The percentage of immigrant in a population.</t>
+          <t>A immigrant population statistic that is the percentage of people that are a immigrant in the population.</t>
         </is>
       </c>
       <c r="D496" t="inlineStr">
@@ -23878,7 +23878,7 @@
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>The proportion of immigrant in a population.</t>
+          <t>A immigrant population statistic that is the proportion of people that are a immigrant in the population.</t>
         </is>
       </c>
       <c r="D497" t="inlineStr">
@@ -23980,7 +23980,7 @@
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>The percentage of in a legal marriage or union in a population.</t>
+          <t>A in a legal marriage or union population statistic that is the percentage of people that are in a legal marriage or union in the population.</t>
         </is>
       </c>
       <c r="D499" t="inlineStr">
@@ -24031,7 +24031,7 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>The proportion of in a legal marriage or union in a population.</t>
+          <t>A in a legal marriage or union population statistic that is the proportion of people that are in a legal marriage or union in the population.</t>
         </is>
       </c>
       <c r="D500" t="inlineStr">
@@ -24133,7 +24133,7 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>The percentage of in a stable or common law relationship in a population.</t>
+          <t>A in a stable or common law relationship population statistic that is the percentage of people that are in a stable or common law relationship in the population.</t>
         </is>
       </c>
       <c r="D502" t="inlineStr">
@@ -24184,7 +24184,7 @@
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>The proportion of in a stable or common law relationship in a population.</t>
+          <t>A in a stable or common law relationship population statistic that is the proportion of people that are in a stable or common law relationship in the population.</t>
         </is>
       </c>
       <c r="D503" t="inlineStr">
@@ -24286,7 +24286,7 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>The percentage of in permanent employment in a population.</t>
+          <t>A in permanent employment population statistic that is the percentage of people that are in permanent employment in the population.</t>
         </is>
       </c>
       <c r="D505" t="inlineStr">
@@ -24337,7 +24337,7 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>The proportion of in permanent employment in a population.</t>
+          <t>A in permanent employment population statistic that is the proportion of people that are in permanent employment in the population.</t>
         </is>
       </c>
       <c r="D506" t="inlineStr">
@@ -24439,7 +24439,7 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>The percentage of in short term or temporary employment with known conditions in a population.</t>
+          <t>A in short term or temporary employment with known conditions population statistic that is the percentage of people that are in short term or temporary employment with known conditions in the population.</t>
         </is>
       </c>
       <c r="D508" t="inlineStr">
@@ -24490,7 +24490,7 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>The proportion of in short term or temporary employment with known conditions in a population.</t>
+          <t>A in short term or temporary employment with known conditions population statistic that is the proportion of people that are in short term or temporary employment with known conditions in the population.</t>
         </is>
       </c>
       <c r="D509" t="inlineStr">
@@ -24592,7 +24592,7 @@
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>The percentage of in uncertain employment in a population.</t>
+          <t>A in uncertain employment population statistic that is the percentage of people that are in uncertain employment in the population.</t>
         </is>
       </c>
       <c r="D511" t="inlineStr">
@@ -24643,7 +24643,7 @@
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>The proportion of in uncertain employment in a population.</t>
+          <t>A in uncertain employment population statistic that is the proportion of people that are in uncertain employment in the population.</t>
         </is>
       </c>
       <c r="D512" t="inlineStr">
@@ -24745,7 +24745,7 @@
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>The percentage of income-related welfare benefit in a population.</t>
+          <t>A income-related welfare benefit population statistic that is the percentage of people that have income-related welfare benefit in the population.</t>
         </is>
       </c>
       <c r="D514" t="inlineStr">
@@ -24796,7 +24796,7 @@
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>The proportion of income-related welfare benefit in a population.</t>
+          <t>A income-related welfare benefit population statistic that is the proportion of people that have income-related welfare benefit in the population.</t>
         </is>
       </c>
       <c r="D515" t="inlineStr">
@@ -24898,7 +24898,7 @@
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>The percentage of independently wealthy status in a population.</t>
+          <t>A independently wealthy status population statistic that is the percentage of people that have independently wealthy status in the population.</t>
         </is>
       </c>
       <c r="D517" t="inlineStr">
@@ -24949,7 +24949,7 @@
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>The proportion of independently wealthy status in a population.</t>
+          <t>A independently wealthy status population statistic that is the proportion of people that have independently wealthy status in the population.</t>
         </is>
       </c>
       <c r="D518" t="inlineStr">
@@ -25051,7 +25051,7 @@
       </c>
       <c r="C520" t="inlineStr">
         <is>
-          <t>The mean of individual human behaviour in a population.</t>
+          <t>A individual human behaviour population statistic that is the mean value of individual human behaviour in the population.</t>
         </is>
       </c>
       <c r="D520" t="inlineStr">
@@ -25102,7 +25102,7 @@
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>The minimum of individual human behaviour in a population.</t>
+          <t>A individual human behaviour population statistic that is the minimum value of individual human behaviour in the population.</t>
         </is>
       </c>
       <c r="D521" t="inlineStr">
@@ -25153,7 +25153,7 @@
       </c>
       <c r="C522" t="inlineStr">
         <is>
-          <t>The maximum of individual human behaviour in a population.</t>
+          <t>A individual human behaviour population statistic that is the maximum value of individual human behaviour in the population.</t>
         </is>
       </c>
       <c r="D522" t="inlineStr">
@@ -25204,7 +25204,7 @@
       </c>
       <c r="C523" t="inlineStr">
         <is>
-          <t>The median of individual human behaviour in a population.</t>
+          <t>A individual human behaviour population statistic that is the median value of individual human behaviour in the population.</t>
         </is>
       </c>
       <c r="D523" t="inlineStr">
@@ -25255,7 +25255,7 @@
       </c>
       <c r="C524" t="inlineStr">
         <is>
-          <t>The percentage of individual human behaviour in a population.</t>
+          <t>A individual human behaviour population statistic that is the percentage value of individual human behaviour in the population.</t>
         </is>
       </c>
       <c r="D524" t="inlineStr">
@@ -25306,7 +25306,7 @@
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>The proportion of individual human behaviour in a population.</t>
+          <t>A individual human behaviour population statistic that is the proportion of individuals having a individual human behaviour in the population.</t>
         </is>
       </c>
       <c r="D525" t="inlineStr">
@@ -25408,7 +25408,7 @@
       </c>
       <c r="C527" t="inlineStr">
         <is>
-          <t>The mean of individual income in a population.</t>
+          <t>A individual income population statistic that is the mean value of individual income in the population.</t>
         </is>
       </c>
       <c r="D527" t="inlineStr">
@@ -25459,7 +25459,7 @@
       </c>
       <c r="C528" t="inlineStr">
         <is>
-          <t>The minimum of individual income in a population.</t>
+          <t>A individual income population statistic that is the minimum value of individual income in the population.</t>
         </is>
       </c>
       <c r="D528" t="inlineStr">
@@ -25510,7 +25510,7 @@
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>The maximum of individual income in a population.</t>
+          <t>A individual income population statistic that is the maximum value of individual income in the population.</t>
         </is>
       </c>
       <c r="D529" t="inlineStr">
@@ -25561,7 +25561,7 @@
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>The median of individual income in a population.</t>
+          <t>A individual income population statistic that is the median value of individual income in the population.</t>
         </is>
       </c>
       <c r="D530" t="inlineStr">
@@ -25612,7 +25612,7 @@
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>The percentage of individual income in a population.</t>
+          <t>A individual income population statistic that is the percentage value of individual income in the population.</t>
         </is>
       </c>
       <c r="D531" t="inlineStr">
@@ -25663,7 +25663,7 @@
       </c>
       <c r="C532" t="inlineStr">
         <is>
-          <t>The proportion of individual income in a population.</t>
+          <t>A individual income population statistic that is the proportion of individuals having a individual income in the population.</t>
         </is>
       </c>
       <c r="D532" t="inlineStr">
@@ -25765,7 +25765,7 @@
       </c>
       <c r="C534" t="inlineStr">
         <is>
-          <t>The percentage of influencer role in a population.</t>
+          <t>A influencer role population statistic that is the percentage of people that have a influencer role in the population.</t>
         </is>
       </c>
       <c r="D534" t="inlineStr">
@@ -25816,7 +25816,7 @@
       </c>
       <c r="C535" t="inlineStr">
         <is>
-          <t>The proportion of influencer role in a population.</t>
+          <t>A influencer role population statistic that is the proportion of people that have a influencer role in the population.</t>
         </is>
       </c>
       <c r="D535" t="inlineStr">
@@ -25918,7 +25918,7 @@
       </c>
       <c r="C537" t="inlineStr">
         <is>
-          <t>The percentage of informal education student role in a population.</t>
+          <t>A informal education student role population statistic that is the percentage of people that have a informal education student role in the population.</t>
         </is>
       </c>
       <c r="D537" t="inlineStr">
@@ -25969,7 +25969,7 @@
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>The proportion of informal education student role in a population.</t>
+          <t>A informal education student role population statistic that is the proportion of people that have a informal education student role in the population.</t>
         </is>
       </c>
       <c r="D538" t="inlineStr">
@@ -26071,7 +26071,7 @@
       </c>
       <c r="C540" t="inlineStr">
         <is>
-          <t>The percentage of inpatient role in a population.</t>
+          <t>A inpatient role population statistic that is the percentage of people that have a inpatient role in the population.</t>
         </is>
       </c>
       <c r="D540" t="inlineStr">
@@ -26122,7 +26122,7 @@
       </c>
       <c r="C541" t="inlineStr">
         <is>
-          <t>The proportion of inpatient role in a population.</t>
+          <t>A inpatient role population statistic that is the proportion of people that have a inpatient role in the population.</t>
         </is>
       </c>
       <c r="D541" t="inlineStr">
@@ -26224,7 +26224,7 @@
       </c>
       <c r="C543" t="inlineStr">
         <is>
-          <t>The percentage of insured party role in a population.</t>
+          <t>A insured party role population statistic that is the percentage of people that have a insured party role in the population.</t>
         </is>
       </c>
       <c r="D543" t="inlineStr">
@@ -26275,7 +26275,7 @@
       </c>
       <c r="C544" t="inlineStr">
         <is>
-          <t>The proportion of insured party role in a population.</t>
+          <t>A insured party role population statistic that is the proportion of people that have a insured party role in the population.</t>
         </is>
       </c>
       <c r="D544" t="inlineStr">
@@ -26377,7 +26377,7 @@
       </c>
       <c r="C546" t="inlineStr">
         <is>
-          <t>The percentage of interpersonal role in a population.</t>
+          <t>A interpersonal role population statistic that is the percentage of people that have a interpersonal role in the population.</t>
         </is>
       </c>
       <c r="D546" t="inlineStr">
@@ -26428,7 +26428,7 @@
       </c>
       <c r="C547" t="inlineStr">
         <is>
-          <t>The proportion of interpersonal role in a population.</t>
+          <t>A interpersonal role population statistic that is the proportion of people that have a interpersonal role in the population.</t>
         </is>
       </c>
       <c r="D547" t="inlineStr">
@@ -26530,7 +26530,7 @@
       </c>
       <c r="C549" t="inlineStr">
         <is>
-          <t>The mean of language proficiency in a population.</t>
+          <t>A language proficiency population statistic that is the mean value of language proficiency in the population.</t>
         </is>
       </c>
       <c r="D549" t="inlineStr">
@@ -26581,7 +26581,7 @@
       </c>
       <c r="C550" t="inlineStr">
         <is>
-          <t>The minimum of language proficiency in a population.</t>
+          <t>A language proficiency population statistic that is the minimum value of language proficiency in the population.</t>
         </is>
       </c>
       <c r="D550" t="inlineStr">
@@ -26632,7 +26632,7 @@
       </c>
       <c r="C551" t="inlineStr">
         <is>
-          <t>The maximum of language proficiency in a population.</t>
+          <t>A language proficiency population statistic that is the maximum value of language proficiency in the population.</t>
         </is>
       </c>
       <c r="D551" t="inlineStr">
@@ -26683,7 +26683,7 @@
       </c>
       <c r="C552" t="inlineStr">
         <is>
-          <t>The median of language proficiency in a population.</t>
+          <t>A language proficiency population statistic that is the median value of language proficiency in the population.</t>
         </is>
       </c>
       <c r="D552" t="inlineStr">
@@ -26734,7 +26734,7 @@
       </c>
       <c r="C553" t="inlineStr">
         <is>
-          <t>The percentage of language proficiency in a population.</t>
+          <t>A language proficiency population statistic that is the percentage value of language proficiency in the population.</t>
         </is>
       </c>
       <c r="D553" t="inlineStr">
@@ -26785,7 +26785,7 @@
       </c>
       <c r="C554" t="inlineStr">
         <is>
-          <t>The proportion of language proficiency in a population.</t>
+          <t>A language proficiency population statistic that is the proportion of individuals having a language proficiency in the population.</t>
         </is>
       </c>
       <c r="D554" t="inlineStr">
@@ -26887,7 +26887,7 @@
       </c>
       <c r="C556" t="inlineStr">
         <is>
-          <t>The mean of linguistic capability in a population.</t>
+          <t>A linguistic capability population statistic that is the mean value of linguistic capability in the population.</t>
         </is>
       </c>
       <c r="D556" t="inlineStr">
@@ -26938,7 +26938,7 @@
       </c>
       <c r="C557" t="inlineStr">
         <is>
-          <t>The minimum of linguistic capability in a population.</t>
+          <t>A linguistic capability population statistic that is the minimum value of linguistic capability in the population.</t>
         </is>
       </c>
       <c r="D557" t="inlineStr">
@@ -26989,7 +26989,7 @@
       </c>
       <c r="C558" t="inlineStr">
         <is>
-          <t>The maximum of linguistic capability in a population.</t>
+          <t>A linguistic capability population statistic that is the maximum value of linguistic capability in the population.</t>
         </is>
       </c>
       <c r="D558" t="inlineStr">
@@ -27040,7 +27040,7 @@
       </c>
       <c r="C559" t="inlineStr">
         <is>
-          <t>The median of linguistic capability in a population.</t>
+          <t>A linguistic capability population statistic that is the median value of linguistic capability in the population.</t>
         </is>
       </c>
       <c r="D559" t="inlineStr">
@@ -27091,7 +27091,7 @@
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>The percentage of linguistic capability in a population.</t>
+          <t>A linguistic capability population statistic that is the percentage value of linguistic capability in the population.</t>
         </is>
       </c>
       <c r="D560" t="inlineStr">
@@ -27142,7 +27142,7 @@
       </c>
       <c r="C561" t="inlineStr">
         <is>
-          <t>The proportion of linguistic capability in a population.</t>
+          <t>A linguistic capability population statistic that is the proportion of individuals having a linguistic capability in the population.</t>
         </is>
       </c>
       <c r="D561" t="inlineStr">
@@ -27244,7 +27244,7 @@
       </c>
       <c r="C563" t="inlineStr">
         <is>
-          <t>The percentage of long-term disabled in a population.</t>
+          <t>A long-term disabled population statistic that is the percentage of people that are long-term disabled in the population.</t>
         </is>
       </c>
       <c r="D563" t="inlineStr">
@@ -27295,7 +27295,7 @@
       </c>
       <c r="C564" t="inlineStr">
         <is>
-          <t>The proportion of long-term disabled in a population.</t>
+          <t>A long-term disabled population statistic that is the proportion of people that are long-term disabled in the population.</t>
         </is>
       </c>
       <c r="D564" t="inlineStr">
@@ -27397,7 +27397,7 @@
       </c>
       <c r="C566" t="inlineStr">
         <is>
-          <t>The percentage of male biological sex in a population.</t>
+          <t>A male biological sex population statistic that is the percentage of people that have a male biological sex in the population.</t>
         </is>
       </c>
       <c r="D566" t="inlineStr">
@@ -27448,7 +27448,7 @@
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>The proportion of male biological sex in a population.</t>
+          <t>A male biological sex population statistic that is the proportion of people that have a male biological sex in the population.</t>
         </is>
       </c>
       <c r="D567" t="inlineStr">
@@ -27550,7 +27550,7 @@
       </c>
       <c r="C569" t="inlineStr">
         <is>
-          <t>The percentage of male gender in a population.</t>
+          <t>A male gender population statistic that is the percentage of people that have a male gender in the population.</t>
         </is>
       </c>
       <c r="D569" t="inlineStr">
@@ -27601,7 +27601,7 @@
       </c>
       <c r="C570" t="inlineStr">
         <is>
-          <t>The proportion of male gender in a population.</t>
+          <t>A male gender population statistic that is the proportion of people that have a male gender in the population.</t>
         </is>
       </c>
       <c r="D570" t="inlineStr">
@@ -27703,7 +27703,7 @@
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>The percentage of masters student role in a population.</t>
+          <t>A masters student role population statistic that is the percentage of people that have a masters student role in the population.</t>
         </is>
       </c>
       <c r="D572" t="inlineStr">
@@ -27754,7 +27754,7 @@
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>The proportion of masters student role in a population.</t>
+          <t>A masters student role population statistic that is the proportion of people that have a masters student role in the population.</t>
         </is>
       </c>
       <c r="D573" t="inlineStr">
@@ -27856,7 +27856,7 @@
       </c>
       <c r="C575" t="inlineStr">
         <is>
-          <t>The percentage of medication use status in a population.</t>
+          <t>A medication use status population statistic that is the percentage of people that have medication use status in the population.</t>
         </is>
       </c>
       <c r="D575" t="inlineStr">
@@ -27907,7 +27907,7 @@
       </c>
       <c r="C576" t="inlineStr">
         <is>
-          <t>The proportion of medication use status in a population.</t>
+          <t>A medication use status population statistic that is the proportion of people that have medication use status in the population.</t>
         </is>
       </c>
       <c r="D576" t="inlineStr">
@@ -28009,7 +28009,7 @@
       </c>
       <c r="C578" t="inlineStr">
         <is>
-          <t>The percentage of member of a multi-person household in a population.</t>
+          <t>A member of a multi-person household population statistic that is the percentage of people that are a member of a multi-person household in the population.</t>
         </is>
       </c>
       <c r="D578" t="inlineStr">
@@ -28060,7 +28060,7 @@
       </c>
       <c r="C579" t="inlineStr">
         <is>
-          <t>The proportion of member of a multi-person household in a population.</t>
+          <t>A member of a multi-person household population statistic that is the proportion of people that are a member of a multi-person household in the population.</t>
         </is>
       </c>
       <c r="D579" t="inlineStr">
@@ -28162,7 +28162,7 @@
       </c>
       <c r="C581" t="inlineStr">
         <is>
-          <t>The percentage of member of a multi-person household all related in a population.</t>
+          <t>A member of a multi-person household all related population statistic that is the percentage of people that are a member of a multi-person household all related in the population.</t>
         </is>
       </c>
       <c r="D581" t="inlineStr">
@@ -28213,7 +28213,7 @@
       </c>
       <c r="C582" t="inlineStr">
         <is>
-          <t>The proportion of member of a multi-person household all related in a population.</t>
+          <t>A member of a multi-person household all related population statistic that is the proportion of people that are a member of a multi-person household all related in the population.</t>
         </is>
       </c>
       <c r="D582" t="inlineStr">
@@ -28315,7 +28315,7 @@
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>The percentage of member of a multi-person household not related in a population.</t>
+          <t>A member of a multi-person household not related population statistic that is the percentage of people that are a member of a multi-person household not related in the population.</t>
         </is>
       </c>
       <c r="D584" t="inlineStr">
@@ -28366,7 +28366,7 @@
       </c>
       <c r="C585" t="inlineStr">
         <is>
-          <t>The proportion of member of a multi-person household not related in a population.</t>
+          <t>A member of a multi-person household not related population statistic that is the proportion of people that are a member of a multi-person household not related in the population.</t>
         </is>
       </c>
       <c r="D585" t="inlineStr">
@@ -28468,7 +28468,7 @@
       </c>
       <c r="C587" t="inlineStr">
         <is>
-          <t>The percentage of member of a multi-person household some related in a population.</t>
+          <t>A member of a multi-person household some related population statistic that is the percentage of people that are a member of a multi-person household some related in the population.</t>
         </is>
       </c>
       <c r="D587" t="inlineStr">
@@ -28519,7 +28519,7 @@
       </c>
       <c r="C588" t="inlineStr">
         <is>
-          <t>The proportion of member of a multi-person household some related in a population.</t>
+          <t>A member of a multi-person household some related population statistic that is the proportion of people that are a member of a multi-person household some related in the population.</t>
         </is>
       </c>
       <c r="D588" t="inlineStr">
@@ -28621,7 +28621,7 @@
       </c>
       <c r="C590" t="inlineStr">
         <is>
-          <t>The percentage of member of a multi-person multi-generational household in a population.</t>
+          <t>A member of a multi-person multi-generational household population statistic that is the percentage of people that are a member of a multi-person multi-generational household in the population.</t>
         </is>
       </c>
       <c r="D590" t="inlineStr">
@@ -28672,7 +28672,7 @@
       </c>
       <c r="C591" t="inlineStr">
         <is>
-          <t>The proportion of member of a multi-person multi-generational household in a population.</t>
+          <t>A member of a multi-person multi-generational household population statistic that is the proportion of people that are a member of a multi-person multi-generational household in the population.</t>
         </is>
       </c>
       <c r="D591" t="inlineStr">
@@ -28774,7 +28774,7 @@
       </c>
       <c r="C593" t="inlineStr">
         <is>
-          <t>The percentage of member of a one person household in a population.</t>
+          <t>A member of a one person household population statistic that is the percentage of people that are a member of a one person household in the population.</t>
         </is>
       </c>
       <c r="D593" t="inlineStr">
@@ -28825,7 +28825,7 @@
       </c>
       <c r="C594" t="inlineStr">
         <is>
-          <t>The proportion of member of a one person household in a population.</t>
+          <t>A member of a one person household population statistic that is the proportion of people that are a member of a one person household in the population.</t>
         </is>
       </c>
       <c r="D594" t="inlineStr">
@@ -28927,7 +28927,7 @@
       </c>
       <c r="C596" t="inlineStr">
         <is>
-          <t>The mean of mental capability in a population.</t>
+          <t>A mental capability population statistic that is the mean value of mental capability in the population.</t>
         </is>
       </c>
       <c r="D596" t="inlineStr">
@@ -28978,7 +28978,7 @@
       </c>
       <c r="C597" t="inlineStr">
         <is>
-          <t>The minimum of mental capability in a population.</t>
+          <t>A mental capability population statistic that is the minimum value of mental capability in the population.</t>
         </is>
       </c>
       <c r="D597" t="inlineStr">
@@ -29029,7 +29029,7 @@
       </c>
       <c r="C598" t="inlineStr">
         <is>
-          <t>The maximum of mental capability in a population.</t>
+          <t>A mental capability population statistic that is the maximum value of mental capability in the population.</t>
         </is>
       </c>
       <c r="D598" t="inlineStr">
@@ -29080,7 +29080,7 @@
       </c>
       <c r="C599" t="inlineStr">
         <is>
-          <t>The median of mental capability in a population.</t>
+          <t>A mental capability population statistic that is the median value of mental capability in the population.</t>
         </is>
       </c>
       <c r="D599" t="inlineStr">
@@ -29131,7 +29131,7 @@
       </c>
       <c r="C600" t="inlineStr">
         <is>
-          <t>The percentage of mental capability in a population.</t>
+          <t>A mental capability population statistic that is the percentage value of mental capability in the population.</t>
         </is>
       </c>
       <c r="D600" t="inlineStr">
@@ -29182,7 +29182,7 @@
       </c>
       <c r="C601" t="inlineStr">
         <is>
-          <t>The proportion of mental capability in a population.</t>
+          <t>A mental capability population statistic that is the proportion of individuals having a mental capability in the population.</t>
         </is>
       </c>
       <c r="D601" t="inlineStr">
@@ -29284,7 +29284,7 @@
       </c>
       <c r="C603" t="inlineStr">
         <is>
-          <t>The percentage of mother in a population.</t>
+          <t>A mother population statistic that is the percentage of people that are a mother in the population.</t>
         </is>
       </c>
       <c r="D603" t="inlineStr">
@@ -29335,7 +29335,7 @@
       </c>
       <c r="C604" t="inlineStr">
         <is>
-          <t>The proportion of mother in a population.</t>
+          <t>A mother population statistic that is the proportion of people that are a mother in the population.</t>
         </is>
       </c>
       <c r="D604" t="inlineStr">
@@ -29437,7 +29437,7 @@
       </c>
       <c r="C606" t="inlineStr">
         <is>
-          <t>The percentage of nephew in a population.</t>
+          <t>A nephew population statistic that is the percentage of people that are a nephew in the population.</t>
         </is>
       </c>
       <c r="D606" t="inlineStr">
@@ -29488,7 +29488,7 @@
       </c>
       <c r="C607" t="inlineStr">
         <is>
-          <t>The proportion of nephew in a population.</t>
+          <t>A nephew population statistic that is the proportion of people that are a nephew in the population.</t>
         </is>
       </c>
       <c r="D607" t="inlineStr">
@@ -29590,7 +29590,7 @@
       </c>
       <c r="C609" t="inlineStr">
         <is>
-          <t>The percentage of niece in a population.</t>
+          <t>A niece population statistic that is the percentage of people that are a niece in the population.</t>
         </is>
       </c>
       <c r="D609" t="inlineStr">
@@ -29641,7 +29641,7 @@
       </c>
       <c r="C610" t="inlineStr">
         <is>
-          <t>The proportion of niece in a population.</t>
+          <t>A niece population statistic that is the proportion of people that are a niece in the population.</t>
         </is>
       </c>
       <c r="D610" t="inlineStr">
@@ -29743,7 +29743,7 @@
       </c>
       <c r="C612" t="inlineStr">
         <is>
-          <t>The percentage of non-gendered identity in a population.</t>
+          <t>A non-gendered identity population statistic that is the percentage of people that have a non-gendered identity in the population.</t>
         </is>
       </c>
       <c r="D612" t="inlineStr">
@@ -29794,7 +29794,7 @@
       </c>
       <c r="C613" t="inlineStr">
         <is>
-          <t>The proportion of non-gendered identity in a population.</t>
+          <t>A non-gendered identity population statistic that is the proportion of people that have a non-gendered identity in the population.</t>
         </is>
       </c>
       <c r="D613" t="inlineStr">
@@ -29896,7 +29896,7 @@
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>The percentage of nonbinary gender in a population.</t>
+          <t>A nonbinary gender population statistic that is the percentage of people that have a nonbinary gender in the population.</t>
         </is>
       </c>
       <c r="D615" t="inlineStr">
@@ -29947,7 +29947,7 @@
       </c>
       <c r="C616" t="inlineStr">
         <is>
-          <t>The proportion of nonbinary gender in a population.</t>
+          <t>A nonbinary gender population statistic that is the proportion of people that have a nonbinary gender in the population.</t>
         </is>
       </c>
       <c r="D616" t="inlineStr">
@@ -30049,7 +30049,7 @@
       </c>
       <c r="C618" t="inlineStr">
         <is>
-          <t>The percentage of not seeking employment in a population.</t>
+          <t>A not seeking employment population statistic that is the percentage of people that are not seeking employment in the population.</t>
         </is>
       </c>
       <c r="D618" t="inlineStr">
@@ -30100,7 +30100,7 @@
       </c>
       <c r="C619" t="inlineStr">
         <is>
-          <t>The proportion of not seeking employment in a population.</t>
+          <t>A not seeking employment population statistic that is the proportion of people that are not seeking employment in the population.</t>
         </is>
       </c>
       <c r="D619" t="inlineStr">
@@ -30202,7 +30202,7 @@
       </c>
       <c r="C621" t="inlineStr">
         <is>
-          <t>The percentage of not working for health reasons in a population.</t>
+          <t>A not working for health reasons population statistic that is the percentage of people that are not working for health reasons in the population.</t>
         </is>
       </c>
       <c r="D621" t="inlineStr">
@@ -30253,7 +30253,7 @@
       </c>
       <c r="C622" t="inlineStr">
         <is>
-          <t>The proportion of not working for health reasons in a population.</t>
+          <t>A not working for health reasons population statistic that is the proportion of people that are not working for health reasons in the population.</t>
         </is>
       </c>
       <c r="D622" t="inlineStr">
@@ -30355,7 +30355,7 @@
       </c>
       <c r="C624" t="inlineStr">
         <is>
-          <t>The mean of number of years in education completed in a population.</t>
+          <t>A number of years in education completed population statistic that is the mean number of number of years in education completed in the population.</t>
         </is>
       </c>
       <c r="D624" t="inlineStr">
@@ -30406,7 +30406,7 @@
       </c>
       <c r="C625" t="inlineStr">
         <is>
-          <t>The minimum of number of years in education completed in a population.</t>
+          <t>A number of years in education completed population statistic that is the minimum number of number of years in education completed in the population.</t>
         </is>
       </c>
       <c r="D625" t="inlineStr">
@@ -30457,7 +30457,7 @@
       </c>
       <c r="C626" t="inlineStr">
         <is>
-          <t>The maximum of number of years in education completed in a population.</t>
+          <t>A number of years in education completed population statistic that is the maximum number of number of years in education completed in the population.</t>
         </is>
       </c>
       <c r="D626" t="inlineStr">
@@ -30508,7 +30508,7 @@
       </c>
       <c r="C627" t="inlineStr">
         <is>
-          <t>The median of number of years in education completed in a population.</t>
+          <t>A number of years in education completed population statistic that is the median number of number of years in education completed in the population.</t>
         </is>
       </c>
       <c r="D627" t="inlineStr">
@@ -30610,7 +30610,7 @@
       </c>
       <c r="C629" t="inlineStr">
         <is>
-          <t>The percentage of occupational role in a population.</t>
+          <t>A occupational role population statistic that is the percentage of people that have a occupational role in the population.</t>
         </is>
       </c>
       <c r="D629" t="inlineStr">
@@ -30661,7 +30661,7 @@
       </c>
       <c r="C630" t="inlineStr">
         <is>
-          <t>The proportion of occupational role in a population.</t>
+          <t>A occupational role population statistic that is the proportion of people that have a occupational role in the population.</t>
         </is>
       </c>
       <c r="D630" t="inlineStr">
@@ -30763,7 +30763,7 @@
       </c>
       <c r="C632" t="inlineStr">
         <is>
-          <t>The percentage of occupier of employer-provided housing in a population.</t>
+          <t>A occupier of employer-provided housing population statistic that is the percentage of people that are a occupier of employer-provided housing in the population.</t>
         </is>
       </c>
       <c r="D632" t="inlineStr">
@@ -30814,7 +30814,7 @@
       </c>
       <c r="C633" t="inlineStr">
         <is>
-          <t>The proportion of occupier of employer-provided housing in a population.</t>
+          <t>A occupier of employer-provided housing population statistic that is the proportion of people that are a occupier of employer-provided housing in the population.</t>
         </is>
       </c>
       <c r="D633" t="inlineStr">
@@ -30916,7 +30916,7 @@
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>The percentage of organisational role in a population.</t>
+          <t>A organisational role population statistic that is the percentage of people that have a organisational role in the population.</t>
         </is>
       </c>
       <c r="D635" t="inlineStr">
@@ -30967,7 +30967,7 @@
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>The proportion of organisational role in a population.</t>
+          <t>A organisational role population statistic that is the proportion of people that have a organisational role in the population.</t>
         </is>
       </c>
       <c r="D636" t="inlineStr">
@@ -31069,7 +31069,7 @@
       </c>
       <c r="C638" t="inlineStr">
         <is>
-          <t>The percentage of other sexual orientation in a population.</t>
+          <t>A other sexual orientation population statistic that is the percentage of people that have a other sexual orientation in the population.</t>
         </is>
       </c>
       <c r="D638" t="inlineStr">
@@ -31120,7 +31120,7 @@
       </c>
       <c r="C639" t="inlineStr">
         <is>
-          <t>The proportion of other sexual orientation in a population.</t>
+          <t>A other sexual orientation population statistic that is the proportion of people that have a other sexual orientation in the population.</t>
         </is>
       </c>
       <c r="D639" t="inlineStr">
@@ -31222,7 +31222,7 @@
       </c>
       <c r="C641" t="inlineStr">
         <is>
-          <t>The percentage of outpatient role in a population.</t>
+          <t>A outpatient role population statistic that is the percentage of people that have a outpatient role in the population.</t>
         </is>
       </c>
       <c r="D641" t="inlineStr">
@@ -31273,7 +31273,7 @@
       </c>
       <c r="C642" t="inlineStr">
         <is>
-          <t>The proportion of outpatient role in a population.</t>
+          <t>A outpatient role population statistic that is the proportion of people that have a outpatient role in the population.</t>
         </is>
       </c>
       <c r="D642" t="inlineStr">
@@ -31375,7 +31375,7 @@
       </c>
       <c r="C644" t="inlineStr">
         <is>
-          <t>The percentage of owner in a population.</t>
+          <t>A owner population statistic that is the percentage of people that are a owner in the population.</t>
         </is>
       </c>
       <c r="D644" t="inlineStr">
@@ -31426,7 +31426,7 @@
       </c>
       <c r="C645" t="inlineStr">
         <is>
-          <t>The proportion of owner in a population.</t>
+          <t>A owner population statistic that is the proportion of people that are a owner in the population.</t>
         </is>
       </c>
       <c r="D645" t="inlineStr">
@@ -31528,7 +31528,7 @@
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>The percentage of owner-occupier in a population.</t>
+          <t>A owner-occupier population statistic that is the percentage of people that are a owner-occupier in the population.</t>
         </is>
       </c>
       <c r="D647" t="inlineStr">
@@ -31579,7 +31579,7 @@
       </c>
       <c r="C648" t="inlineStr">
         <is>
-          <t>The proportion of owner-occupier in a population.</t>
+          <t>A owner-occupier population statistic that is the proportion of people that are a owner-occupier in the population.</t>
         </is>
       </c>
       <c r="D648" t="inlineStr">
@@ -31681,7 +31681,7 @@
       </c>
       <c r="C650" t="inlineStr">
         <is>
-          <t>The percentage of parent in a population.</t>
+          <t>A parent population statistic that is the percentage of people that are a parent in the population.</t>
         </is>
       </c>
       <c r="D650" t="inlineStr">
@@ -31732,7 +31732,7 @@
       </c>
       <c r="C651" t="inlineStr">
         <is>
-          <t>The proportion of parent in a population.</t>
+          <t>A parent population statistic that is the proportion of people that are a parent in the population.</t>
         </is>
       </c>
       <c r="D651" t="inlineStr">
@@ -31834,7 +31834,7 @@
       </c>
       <c r="C653" t="inlineStr">
         <is>
-          <t>The percentage of parental role in a population.</t>
+          <t>A parental role population statistic that is the percentage of people that have a parental role in the population.</t>
         </is>
       </c>
       <c r="D653" t="inlineStr">
@@ -31885,7 +31885,7 @@
       </c>
       <c r="C654" t="inlineStr">
         <is>
-          <t>The proportion of parental role in a population.</t>
+          <t>A parental role population statistic that is the proportion of people that have a parental role in the population.</t>
         </is>
       </c>
       <c r="D654" t="inlineStr">
@@ -31987,7 +31987,7 @@
       </c>
       <c r="C656" t="inlineStr">
         <is>
-          <t>The mean of past behaviour  in a population.</t>
+          <t>A past behaviour  population statistic that is the mean value of past behaviour  in the population.</t>
         </is>
       </c>
       <c r="D656" t="inlineStr">
@@ -32038,7 +32038,7 @@
       </c>
       <c r="C657" t="inlineStr">
         <is>
-          <t>The minimum of past behaviour  in a population.</t>
+          <t>A past behaviour  population statistic that is the minimum value of past behaviour  in the population.</t>
         </is>
       </c>
       <c r="D657" t="inlineStr">
@@ -32089,7 +32089,7 @@
       </c>
       <c r="C658" t="inlineStr">
         <is>
-          <t>The maximum of past behaviour  in a population.</t>
+          <t>A past behaviour  population statistic that is the maximum value of past behaviour  in the population.</t>
         </is>
       </c>
       <c r="D658" t="inlineStr">
@@ -32140,7 +32140,7 @@
       </c>
       <c r="C659" t="inlineStr">
         <is>
-          <t>The median of past behaviour  in a population.</t>
+          <t>A past behaviour  population statistic that is the median value of past behaviour  in the population.</t>
         </is>
       </c>
       <c r="D659" t="inlineStr">
@@ -32191,7 +32191,7 @@
       </c>
       <c r="C660" t="inlineStr">
         <is>
-          <t>The percentage of past behaviour  in a population.</t>
+          <t>A past behaviour  population statistic that is the percentage value of past behaviour  in the population.</t>
         </is>
       </c>
       <c r="D660" t="inlineStr">
@@ -32242,7 +32242,7 @@
       </c>
       <c r="C661" t="inlineStr">
         <is>
-          <t>The proportion of past behaviour  in a population.</t>
+          <t>A past behaviour  population statistic that is the proportion of individuals having a past behaviour  in the population.</t>
         </is>
       </c>
       <c r="D661" t="inlineStr">
@@ -32344,7 +32344,7 @@
       </c>
       <c r="C663" t="inlineStr">
         <is>
-          <t>The percentage of patient role in a population.</t>
+          <t>A patient role population statistic that is the percentage of people that have a patient role in the population.</t>
         </is>
       </c>
       <c r="D663" t="inlineStr">
@@ -32395,7 +32395,7 @@
       </c>
       <c r="C664" t="inlineStr">
         <is>
-          <t>The proportion of patient role in a population.</t>
+          <t>A patient role population statistic that is the proportion of people that have a patient role in the population.</t>
         </is>
       </c>
       <c r="D664" t="inlineStr">
@@ -32497,7 +32497,7 @@
       </c>
       <c r="C666" t="inlineStr">
         <is>
-          <t>The mean of personal history of behavioural lapse in a population.</t>
+          <t>A personal history of behavioural lapse population statistic that is the mean value of personal history of behavioural lapse in the population.</t>
         </is>
       </c>
       <c r="D666" t="inlineStr">
@@ -32548,7 +32548,7 @@
       </c>
       <c r="C667" t="inlineStr">
         <is>
-          <t>The minimum of personal history of behavioural lapse in a population.</t>
+          <t>A personal history of behavioural lapse population statistic that is the minimum value of personal history of behavioural lapse in the population.</t>
         </is>
       </c>
       <c r="D667" t="inlineStr">
@@ -32599,7 +32599,7 @@
       </c>
       <c r="C668" t="inlineStr">
         <is>
-          <t>The maximum of personal history of behavioural lapse in a population.</t>
+          <t>A personal history of behavioural lapse population statistic that is the maximum value of personal history of behavioural lapse in the population.</t>
         </is>
       </c>
       <c r="D668" t="inlineStr">
@@ -32650,7 +32650,7 @@
       </c>
       <c r="C669" t="inlineStr">
         <is>
-          <t>The median of personal history of behavioural lapse in a population.</t>
+          <t>A personal history of behavioural lapse population statistic that is the median value of personal history of behavioural lapse in the population.</t>
         </is>
       </c>
       <c r="D669" t="inlineStr">
@@ -32701,7 +32701,7 @@
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>The percentage of personal history of behavioural lapse in a population.</t>
+          <t>A personal history of behavioural lapse population statistic that is the percentage value of personal history of behavioural lapse in the population.</t>
         </is>
       </c>
       <c r="D670" t="inlineStr">
@@ -32752,7 +32752,7 @@
       </c>
       <c r="C671" t="inlineStr">
         <is>
-          <t>The proportion of personal history of behavioural lapse in a population.</t>
+          <t>A personal history of behavioural lapse population statistic that is the proportion of individuals having a personal history of behavioural lapse in the population.</t>
         </is>
       </c>
       <c r="D671" t="inlineStr">
@@ -32854,7 +32854,7 @@
       </c>
       <c r="C673" t="inlineStr">
         <is>
-          <t>The mean of personal history of events that influence behaviour  in a population.</t>
+          <t>A personal history of events that influence behaviour  population statistic that is the mean value of personal history of events that influence behaviour  in the population.</t>
         </is>
       </c>
       <c r="D673" t="inlineStr">
@@ -32905,7 +32905,7 @@
       </c>
       <c r="C674" t="inlineStr">
         <is>
-          <t>The minimum of personal history of events that influence behaviour  in a population.</t>
+          <t>A personal history of events that influence behaviour  population statistic that is the minimum value of personal history of events that influence behaviour  in the population.</t>
         </is>
       </c>
       <c r="D674" t="inlineStr">
@@ -32956,7 +32956,7 @@
       </c>
       <c r="C675" t="inlineStr">
         <is>
-          <t>The maximum of personal history of events that influence behaviour  in a population.</t>
+          <t>A personal history of events that influence behaviour  population statistic that is the maximum value of personal history of events that influence behaviour  in the population.</t>
         </is>
       </c>
       <c r="D675" t="inlineStr">
@@ -33007,7 +33007,7 @@
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>The median of personal history of events that influence behaviour  in a population.</t>
+          <t>A personal history of events that influence behaviour  population statistic that is the median value of personal history of events that influence behaviour  in the population.</t>
         </is>
       </c>
       <c r="D676" t="inlineStr">
@@ -33058,7 +33058,7 @@
       </c>
       <c r="C677" t="inlineStr">
         <is>
-          <t>The percentage of personal history of events that influence behaviour  in a population.</t>
+          <t>A personal history of events that influence behaviour  population statistic that is the percentage value of personal history of events that influence behaviour  in the population.</t>
         </is>
       </c>
       <c r="D677" t="inlineStr">
@@ -33109,7 +33109,7 @@
       </c>
       <c r="C678" t="inlineStr">
         <is>
-          <t>The proportion of personal history of events that influence behaviour  in a population.</t>
+          <t>A personal history of events that influence behaviour  population statistic that is the proportion of individuals having a personal history of events that influence behaviour  in the population.</t>
         </is>
       </c>
       <c r="D678" t="inlineStr">
@@ -33211,7 +33211,7 @@
       </c>
       <c r="C680" t="inlineStr">
         <is>
-          <t>The mean of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome population statistic that is the mean value of personal history of intervention exposure for the same outcome in the population.</t>
         </is>
       </c>
       <c r="D680" t="inlineStr">
@@ -33262,7 +33262,7 @@
       </c>
       <c r="C681" t="inlineStr">
         <is>
-          <t>The minimum of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome population statistic that is the minimum value of personal history of intervention exposure for the same outcome in the population.</t>
         </is>
       </c>
       <c r="D681" t="inlineStr">
@@ -33313,7 +33313,7 @@
       </c>
       <c r="C682" t="inlineStr">
         <is>
-          <t>The maximum of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome population statistic that is the maximum value of personal history of intervention exposure for the same outcome in the population.</t>
         </is>
       </c>
       <c r="D682" t="inlineStr">
@@ -33364,7 +33364,7 @@
       </c>
       <c r="C683" t="inlineStr">
         <is>
-          <t>The median of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome population statistic that is the median value of personal history of intervention exposure for the same outcome in the population.</t>
         </is>
       </c>
       <c r="D683" t="inlineStr">
@@ -33415,7 +33415,7 @@
       </c>
       <c r="C684" t="inlineStr">
         <is>
-          <t>The percentage of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome population statistic that is the percentage value of personal history of intervention exposure for the same outcome in the population.</t>
         </is>
       </c>
       <c r="D684" t="inlineStr">
@@ -33466,7 +33466,7 @@
       </c>
       <c r="C685" t="inlineStr">
         <is>
-          <t>The proportion of personal history of intervention exposure for the same outcome in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome population statistic that is the proportion of individuals having a personal history of intervention exposure for the same outcome in the population.</t>
         </is>
       </c>
       <c r="D685" t="inlineStr">
@@ -33568,7 +33568,7 @@
       </c>
       <c r="C687" t="inlineStr">
         <is>
-          <t>The mean of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome behaviour population statistic that is the mean value of personal history of intervention exposure for the same outcome behaviour in the population.</t>
         </is>
       </c>
       <c r="D687" t="inlineStr">
@@ -33619,7 +33619,7 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>The minimum of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome behaviour population statistic that is the minimum value of personal history of intervention exposure for the same outcome behaviour in the population.</t>
         </is>
       </c>
       <c r="D688" t="inlineStr">
@@ -33670,7 +33670,7 @@
       </c>
       <c r="C689" t="inlineStr">
         <is>
-          <t>The maximum of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome behaviour population statistic that is the maximum value of personal history of intervention exposure for the same outcome behaviour in the population.</t>
         </is>
       </c>
       <c r="D689" t="inlineStr">
@@ -33721,7 +33721,7 @@
       </c>
       <c r="C690" t="inlineStr">
         <is>
-          <t>The median of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome behaviour population statistic that is the median value of personal history of intervention exposure for the same outcome behaviour in the population.</t>
         </is>
       </c>
       <c r="D690" t="inlineStr">
@@ -33772,7 +33772,7 @@
       </c>
       <c r="C691" t="inlineStr">
         <is>
-          <t>The percentage of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome behaviour population statistic that is the percentage value of personal history of intervention exposure for the same outcome behaviour in the population.</t>
         </is>
       </c>
       <c r="D691" t="inlineStr">
@@ -33823,7 +33823,7 @@
       </c>
       <c r="C692" t="inlineStr">
         <is>
-          <t>The proportion of personal history of intervention exposure for the same outcome behaviour in a population.</t>
+          <t>A personal history of intervention exposure for the same outcome behaviour population statistic that is the proportion of individuals having a personal history of intervention exposure for the same outcome behaviour in the population.</t>
         </is>
       </c>
       <c r="D692" t="inlineStr">
@@ -33925,7 +33925,7 @@
       </c>
       <c r="C694" t="inlineStr">
         <is>
-          <t>The mean of personal history of same intervention exposure in a population.</t>
+          <t>A personal history of same intervention exposure population statistic that is the mean value of personal history of same intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D694" t="inlineStr">
@@ -33976,7 +33976,7 @@
       </c>
       <c r="C695" t="inlineStr">
         <is>
-          <t>The minimum of personal history of same intervention exposure in a population.</t>
+          <t>A personal history of same intervention exposure population statistic that is the minimum value of personal history of same intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D695" t="inlineStr">
@@ -34027,7 +34027,7 @@
       </c>
       <c r="C696" t="inlineStr">
         <is>
-          <t>The maximum of personal history of same intervention exposure in a population.</t>
+          <t>A personal history of same intervention exposure population statistic that is the maximum value of personal history of same intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D696" t="inlineStr">
@@ -34078,7 +34078,7 @@
       </c>
       <c r="C697" t="inlineStr">
         <is>
-          <t>The median of personal history of same intervention exposure in a population.</t>
+          <t>A personal history of same intervention exposure population statistic that is the median value of personal history of same intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D697" t="inlineStr">
@@ -34129,7 +34129,7 @@
       </c>
       <c r="C698" t="inlineStr">
         <is>
-          <t>The percentage of personal history of same intervention exposure in a population.</t>
+          <t>A personal history of same intervention exposure population statistic that is the percentage value of personal history of same intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D698" t="inlineStr">
@@ -34180,7 +34180,7 @@
       </c>
       <c r="C699" t="inlineStr">
         <is>
-          <t>The proportion of personal history of same intervention exposure in a population.</t>
+          <t>A personal history of same intervention exposure population statistic that is the proportion of individuals having a personal history of same intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D699" t="inlineStr">
@@ -34282,7 +34282,7 @@
       </c>
       <c r="C701" t="inlineStr">
         <is>
-          <t>The mean of personal history part of intervention exposure in a population.</t>
+          <t>A personal history part of intervention exposure population statistic that is the mean value of personal history part of intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D701" t="inlineStr">
@@ -34333,7 +34333,7 @@
       </c>
       <c r="C702" t="inlineStr">
         <is>
-          <t>The minimum of personal history part of intervention exposure in a population.</t>
+          <t>A personal history part of intervention exposure population statistic that is the minimum value of personal history part of intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D702" t="inlineStr">
@@ -34384,7 +34384,7 @@
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>The maximum of personal history part of intervention exposure in a population.</t>
+          <t>A personal history part of intervention exposure population statistic that is the maximum value of personal history part of intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D703" t="inlineStr">
@@ -34435,7 +34435,7 @@
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>The median of personal history part of intervention exposure in a population.</t>
+          <t>A personal history part of intervention exposure population statistic that is the median value of personal history part of intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D704" t="inlineStr">
@@ -34486,7 +34486,7 @@
       </c>
       <c r="C705" t="inlineStr">
         <is>
-          <t>The percentage of personal history part of intervention exposure in a population.</t>
+          <t>A personal history part of intervention exposure population statistic that is the percentage value of personal history part of intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D705" t="inlineStr">
@@ -34537,7 +34537,7 @@
       </c>
       <c r="C706" t="inlineStr">
         <is>
-          <t>The proportion of personal history part of intervention exposure in a population.</t>
+          <t>A personal history part of intervention exposure population statistic that is the proportion of individuals having a personal history part of intervention exposure in the population.</t>
         </is>
       </c>
       <c r="D706" t="inlineStr">
@@ -34639,7 +34639,7 @@
       </c>
       <c r="C708" t="inlineStr">
         <is>
-          <t>The mean of personal psychological attribute in a population.</t>
+          <t>A personal psychological attribute population statistic that is the mean value of personal psychological attribute in the population.</t>
         </is>
       </c>
       <c r="D708" t="inlineStr">
@@ -34690,7 +34690,7 @@
       </c>
       <c r="C709" t="inlineStr">
         <is>
-          <t>The minimum of personal psychological attribute in a population.</t>
+          <t>A personal psychological attribute population statistic that is the minimum value of personal psychological attribute in the population.</t>
         </is>
       </c>
       <c r="D709" t="inlineStr">
@@ -34741,7 +34741,7 @@
       </c>
       <c r="C710" t="inlineStr">
         <is>
-          <t>The maximum of personal psychological attribute in a population.</t>
+          <t>A personal psychological attribute population statistic that is the maximum value of personal psychological attribute in the population.</t>
         </is>
       </c>
       <c r="D710" t="inlineStr">
@@ -34792,7 +34792,7 @@
       </c>
       <c r="C711" t="inlineStr">
         <is>
-          <t>The median of personal psychological attribute in a population.</t>
+          <t>A personal psychological attribute population statistic that is the median value of personal psychological attribute in the population.</t>
         </is>
       </c>
       <c r="D711" t="inlineStr">
@@ -34843,7 +34843,7 @@
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>The percentage of personal psychological attribute in a population.</t>
+          <t>A personal psychological attribute population statistic that is the percentage value of personal psychological attribute in the population.</t>
         </is>
       </c>
       <c r="D712" t="inlineStr">
@@ -34894,7 +34894,7 @@
       </c>
       <c r="C713" t="inlineStr">
         <is>
-          <t>The proportion of personal psychological attribute in a population.</t>
+          <t>A personal psychological attribute population statistic that is the proportion of individuals having a personal psychological attribute in the population.</t>
         </is>
       </c>
       <c r="D713" t="inlineStr">
@@ -34996,7 +34996,7 @@
       </c>
       <c r="C715" t="inlineStr">
         <is>
-          <t>The mean of personal vulnerability in a population.</t>
+          <t>A personal vulnerability population statistic that is the mean value of personal vulnerability in the population.</t>
         </is>
       </c>
       <c r="D715" t="inlineStr">
@@ -35047,7 +35047,7 @@
       </c>
       <c r="C716" t="inlineStr">
         <is>
-          <t>The minimum of personal vulnerability in a population.</t>
+          <t>A personal vulnerability population statistic that is the minimum value of personal vulnerability in the population.</t>
         </is>
       </c>
       <c r="D716" t="inlineStr">
@@ -35098,7 +35098,7 @@
       </c>
       <c r="C717" t="inlineStr">
         <is>
-          <t>The maximum of personal vulnerability in a population.</t>
+          <t>A personal vulnerability population statistic that is the maximum value of personal vulnerability in the population.</t>
         </is>
       </c>
       <c r="D717" t="inlineStr">
@@ -35149,7 +35149,7 @@
       </c>
       <c r="C718" t="inlineStr">
         <is>
-          <t>The median of personal vulnerability in a population.</t>
+          <t>A personal vulnerability population statistic that is the median value of personal vulnerability in the population.</t>
         </is>
       </c>
       <c r="D718" t="inlineStr">
@@ -35200,7 +35200,7 @@
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>The percentage of personal vulnerability in a population.</t>
+          <t>A personal vulnerability population statistic that is the percentage value of personal vulnerability in the population.</t>
         </is>
       </c>
       <c r="D719" t="inlineStr">
@@ -35251,7 +35251,7 @@
       </c>
       <c r="C720" t="inlineStr">
         <is>
-          <t>The proportion of personal vulnerability in a population.</t>
+          <t>A personal vulnerability population statistic that is the proportion of individuals having a personal vulnerability in the population.</t>
         </is>
       </c>
       <c r="D720" t="inlineStr">
@@ -35353,7 +35353,7 @@
       </c>
       <c r="C722" t="inlineStr">
         <is>
-          <t>The mean of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A personal vulnerability to harmful behaviour population statistic that is the mean value of personal vulnerability to harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D722" t="inlineStr">
@@ -35404,7 +35404,7 @@
       </c>
       <c r="C723" t="inlineStr">
         <is>
-          <t>The minimum of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A personal vulnerability to harmful behaviour population statistic that is the minimum value of personal vulnerability to harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D723" t="inlineStr">
@@ -35455,7 +35455,7 @@
       </c>
       <c r="C724" t="inlineStr">
         <is>
-          <t>The maximum of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A personal vulnerability to harmful behaviour population statistic that is the maximum value of personal vulnerability to harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D724" t="inlineStr">
@@ -35506,7 +35506,7 @@
       </c>
       <c r="C725" t="inlineStr">
         <is>
-          <t>The median of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A personal vulnerability to harmful behaviour population statistic that is the median value of personal vulnerability to harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D725" t="inlineStr">
@@ -35557,7 +35557,7 @@
       </c>
       <c r="C726" t="inlineStr">
         <is>
-          <t>The percentage of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A personal vulnerability to harmful behaviour population statistic that is the percentage value of personal vulnerability to harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D726" t="inlineStr">
@@ -35608,7 +35608,7 @@
       </c>
       <c r="C727" t="inlineStr">
         <is>
-          <t>The proportion of personal vulnerability to harmful behaviour in a population.</t>
+          <t>A personal vulnerability to harmful behaviour population statistic that is the proportion of individuals having a personal vulnerability to harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D727" t="inlineStr">
@@ -35710,7 +35710,7 @@
       </c>
       <c r="C729" t="inlineStr">
         <is>
-          <t>The percentage of place of residence in a population.</t>
+          <t>A place of residence population statistic that is the percentage of people that have a place of residence in the population.</t>
         </is>
       </c>
       <c r="D729" t="inlineStr">
@@ -35761,7 +35761,7 @@
       </c>
       <c r="C730" t="inlineStr">
         <is>
-          <t>The proportion of place of residence in a population.</t>
+          <t>A place of residence population statistic that is the proportion of people that have a place of residence in the population.</t>
         </is>
       </c>
       <c r="D730" t="inlineStr">
@@ -35863,7 +35863,7 @@
       </c>
       <c r="C732" t="inlineStr">
         <is>
-          <t>The percentage of policy holder role in a population.</t>
+          <t>A policy holder role population statistic that is the percentage of people that have a policy holder role in the population.</t>
         </is>
       </c>
       <c r="D732" t="inlineStr">
@@ -35914,7 +35914,7 @@
       </c>
       <c r="C733" t="inlineStr">
         <is>
-          <t>The proportion of policy holder role in a population.</t>
+          <t>A policy holder role population statistic that is the proportion of people that have a policy holder role in the population.</t>
         </is>
       </c>
       <c r="D733" t="inlineStr">
@@ -36016,7 +36016,7 @@
       </c>
       <c r="C735" t="inlineStr">
         <is>
-          <t>The percentage of preschool student role in a population.</t>
+          <t>A preschool student role population statistic that is the percentage of people that have a preschool student role in the population.</t>
         </is>
       </c>
       <c r="D735" t="inlineStr">
@@ -36067,7 +36067,7 @@
       </c>
       <c r="C736" t="inlineStr">
         <is>
-          <t>The proportion of preschool student role in a population.</t>
+          <t>A preschool student role population statistic that is the proportion of people that have a preschool student role in the population.</t>
         </is>
       </c>
       <c r="D736" t="inlineStr">
@@ -36169,7 +36169,7 @@
       </c>
       <c r="C738" t="inlineStr">
         <is>
-          <t>The mean of protective factor for harmful behaviour in a population.</t>
+          <t>A protective factor for harmful behaviour population statistic that is the mean value of protective factor for harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D738" t="inlineStr">
@@ -36220,7 +36220,7 @@
       </c>
       <c r="C739" t="inlineStr">
         <is>
-          <t>The minimum of protective factor for harmful behaviour in a population.</t>
+          <t>A protective factor for harmful behaviour population statistic that is the minimum value of protective factor for harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D739" t="inlineStr">
@@ -36271,7 +36271,7 @@
       </c>
       <c r="C740" t="inlineStr">
         <is>
-          <t>The maximum of protective factor for harmful behaviour in a population.</t>
+          <t>A protective factor for harmful behaviour population statistic that is the maximum value of protective factor for harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D740" t="inlineStr">
@@ -36322,7 +36322,7 @@
       </c>
       <c r="C741" t="inlineStr">
         <is>
-          <t>The median of protective factor for harmful behaviour in a population.</t>
+          <t>A protective factor for harmful behaviour population statistic that is the median value of protective factor for harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D741" t="inlineStr">
@@ -36373,7 +36373,7 @@
       </c>
       <c r="C742" t="inlineStr">
         <is>
-          <t>The percentage of protective factor for harmful behaviour in a population.</t>
+          <t>A protective factor for harmful behaviour population statistic that is the percentage value of protective factor for harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D742" t="inlineStr">
@@ -36424,7 +36424,7 @@
       </c>
       <c r="C743" t="inlineStr">
         <is>
-          <t>The proportion of protective factor for harmful behaviour in a population.</t>
+          <t>A protective factor for harmful behaviour population statistic that is the proportion of individuals having a protective factor for harmful behaviour in the population.</t>
         </is>
       </c>
       <c r="D743" t="inlineStr">
@@ -36526,7 +36526,7 @@
       </c>
       <c r="C745" t="inlineStr">
         <is>
-          <t>The mean of quantity of valuable material resource owned in a population.</t>
+          <t>A quantity of valuable material resource owned population statistic that is the mean number of quantity of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D745" t="inlineStr">
@@ -36577,7 +36577,7 @@
       </c>
       <c r="C746" t="inlineStr">
         <is>
-          <t>The minimum of quantity of valuable material resource owned in a population.</t>
+          <t>A quantity of valuable material resource owned population statistic that is the minimum number of quantity of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D746" t="inlineStr">
@@ -36628,7 +36628,7 @@
       </c>
       <c r="C747" t="inlineStr">
         <is>
-          <t>The maximum of quantity of valuable material resource owned in a population.</t>
+          <t>A quantity of valuable material resource owned population statistic that is the maximum number of quantity of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D747" t="inlineStr">
@@ -36679,7 +36679,7 @@
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>The median of quantity of valuable material resource owned in a population.</t>
+          <t>A quantity of valuable material resource owned population statistic that is the median number of quantity of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D748" t="inlineStr">
@@ -36781,7 +36781,7 @@
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>The percentage of queer in a population.</t>
+          <t>A queer population statistic that is the percentage of people that are queer in the population.</t>
         </is>
       </c>
       <c r="D750" t="inlineStr">
@@ -36832,7 +36832,7 @@
       </c>
       <c r="C751" t="inlineStr">
         <is>
-          <t>The proportion of queer in a population.</t>
+          <t>A queer population statistic that is the proportion of people that are queer in the population.</t>
         </is>
       </c>
       <c r="D751" t="inlineStr">
@@ -36934,7 +36934,7 @@
       </c>
       <c r="C753" t="inlineStr">
         <is>
-          <t>The percentage of questioning sexual orientation in a population.</t>
+          <t>A questioning sexual orientation population statistic that is the percentage of people that are questioning sexual orientation in the population.</t>
         </is>
       </c>
       <c r="D753" t="inlineStr">
@@ -36985,7 +36985,7 @@
       </c>
       <c r="C754" t="inlineStr">
         <is>
-          <t>The proportion of questioning sexual orientation in a population.</t>
+          <t>A questioning sexual orientation population statistic that is the proportion of people that are questioning sexual orientation in the population.</t>
         </is>
       </c>
       <c r="D754" t="inlineStr">
@@ -37087,7 +37087,7 @@
       </c>
       <c r="C756" t="inlineStr">
         <is>
-          <t>The percentage of relationship status in a population.</t>
+          <t>A relationship status population statistic that is the percentage of people that have a relationship status in the population.</t>
         </is>
       </c>
       <c r="D756" t="inlineStr">
@@ -37138,7 +37138,7 @@
       </c>
       <c r="C757" t="inlineStr">
         <is>
-          <t>The proportion of relationship status in a population.</t>
+          <t>A relationship status population statistic that is the proportion of people that have a relationship status in the population.</t>
         </is>
       </c>
       <c r="D757" t="inlineStr">
@@ -37240,7 +37240,7 @@
       </c>
       <c r="C759" t="inlineStr">
         <is>
-          <t>The percentage of religious group membership in a population.</t>
+          <t>A religious group membership population statistic that is the percentage of people that have a religious group membership in the population.</t>
         </is>
       </c>
       <c r="D759" t="inlineStr">
@@ -37291,7 +37291,7 @@
       </c>
       <c r="C760" t="inlineStr">
         <is>
-          <t>The proportion of religious group membership in a population.</t>
+          <t>A religious group membership population statistic that is the proportion of people that have a religious group membership in the population.</t>
         </is>
       </c>
       <c r="D760" t="inlineStr">
@@ -37393,7 +37393,7 @@
       </c>
       <c r="C762" t="inlineStr">
         <is>
-          <t>The percentage of rent-free occupier in a population.</t>
+          <t>A rent-free occupier population statistic that is the percentage of people that are a rent-free occupier in the population.</t>
         </is>
       </c>
       <c r="D762" t="inlineStr">
@@ -37444,7 +37444,7 @@
       </c>
       <c r="C763" t="inlineStr">
         <is>
-          <t>The proportion of rent-free occupier in a population.</t>
+          <t>A rent-free occupier population statistic that is the proportion of people that are a rent-free occupier in the population.</t>
         </is>
       </c>
       <c r="D763" t="inlineStr">
@@ -37546,7 +37546,7 @@
       </c>
       <c r="C765" t="inlineStr">
         <is>
-          <t>The percentage of rent-free occupier without owner's permission in a population.</t>
+          <t>A rent-free occupier without owner's permission population statistic that is the percentage of people that are a rent-free occupier without owner's permission in the population.</t>
         </is>
       </c>
       <c r="D765" t="inlineStr">
@@ -37597,7 +37597,7 @@
       </c>
       <c r="C766" t="inlineStr">
         <is>
-          <t>The proportion of rent-free occupier without owner's permission in a population.</t>
+          <t>A rent-free occupier without owner's permission population statistic that is the proportion of people that are a rent-free occupier without owner's permission in the population.</t>
         </is>
       </c>
       <c r="D766" t="inlineStr">
@@ -37699,7 +37699,7 @@
       </c>
       <c r="C768" t="inlineStr">
         <is>
-          <t>The percentage of renter in a population.</t>
+          <t>A renter population statistic that is the percentage of people that are a renter in the population.</t>
         </is>
       </c>
       <c r="D768" t="inlineStr">
@@ -37750,7 +37750,7 @@
       </c>
       <c r="C769" t="inlineStr">
         <is>
-          <t>The proportion of renter in a population.</t>
+          <t>A renter population statistic that is the proportion of people that are a renter in the population.</t>
         </is>
       </c>
       <c r="D769" t="inlineStr">
@@ -37852,7 +37852,7 @@
       </c>
       <c r="C771" t="inlineStr">
         <is>
-          <t>The percentage of renter of housing from a social provider in a population.</t>
+          <t>A renter of housing from a social provider population statistic that is the percentage of people that are a renter of housing from a social provider in the population.</t>
         </is>
       </c>
       <c r="D771" t="inlineStr">
@@ -37903,7 +37903,7 @@
       </c>
       <c r="C772" t="inlineStr">
         <is>
-          <t>The proportion of renter of housing from a social provider in a population.</t>
+          <t>A renter of housing from a social provider population statistic that is the proportion of people that are a renter of housing from a social provider in the population.</t>
         </is>
       </c>
       <c r="D772" t="inlineStr">
@@ -38005,7 +38005,7 @@
       </c>
       <c r="C774" t="inlineStr">
         <is>
-          <t>The percentage of residential facility owner in a population.</t>
+          <t>A residential facility owner population statistic that is the percentage of people that are a residential facility owner in the population.</t>
         </is>
       </c>
       <c r="D774" t="inlineStr">
@@ -38056,7 +38056,7 @@
       </c>
       <c r="C775" t="inlineStr">
         <is>
-          <t>The proportion of residential facility owner in a population.</t>
+          <t>A residential facility owner population statistic that is the proportion of people that are a residential facility owner in the population.</t>
         </is>
       </c>
       <c r="D775" t="inlineStr">
@@ -38158,7 +38158,7 @@
       </c>
       <c r="C777" t="inlineStr">
         <is>
-          <t>The percentage of retired status in a population.</t>
+          <t>A retired status population statistic that is the percentage of people that have retired status in the population.</t>
         </is>
       </c>
       <c r="D777" t="inlineStr">
@@ -38209,7 +38209,7 @@
       </c>
       <c r="C778" t="inlineStr">
         <is>
-          <t>The proportion of retired status in a population.</t>
+          <t>A retired status population statistic that is the proportion of people that have retired status in the population.</t>
         </is>
       </c>
       <c r="D778" t="inlineStr">
@@ -38311,7 +38311,7 @@
       </c>
       <c r="C780" t="inlineStr">
         <is>
-          <t>The percentage of school student role in a population.</t>
+          <t>A school student role population statistic that is the percentage of people that have a school student role in the population.</t>
         </is>
       </c>
       <c r="D780" t="inlineStr">
@@ -38362,7 +38362,7 @@
       </c>
       <c r="C781" t="inlineStr">
         <is>
-          <t>The proportion of school student role in a population.</t>
+          <t>A school student role population statistic that is the proportion of people that have a school student role in the population.</t>
         </is>
       </c>
       <c r="D781" t="inlineStr">
@@ -38464,7 +38464,7 @@
       </c>
       <c r="C783" t="inlineStr">
         <is>
-          <t>The percentage of second generation immigrant in a population.</t>
+          <t>A second generation immigrant population statistic that is the percentage of people that are a second generation immigrant in the population.</t>
         </is>
       </c>
       <c r="D783" t="inlineStr">
@@ -38515,7 +38515,7 @@
       </c>
       <c r="C784" t="inlineStr">
         <is>
-          <t>The proportion of second generation immigrant in a population.</t>
+          <t>A second generation immigrant population statistic that is the proportion of people that are a second generation immigrant in the population.</t>
         </is>
       </c>
       <c r="D784" t="inlineStr">
@@ -38617,7 +38617,7 @@
       </c>
       <c r="C786" t="inlineStr">
         <is>
-          <t>The percentage of self employed status in a population.</t>
+          <t>A self employed status population statistic that is the percentage of people that have self employed status in the population.</t>
         </is>
       </c>
       <c r="D786" t="inlineStr">
@@ -38668,7 +38668,7 @@
       </c>
       <c r="C787" t="inlineStr">
         <is>
-          <t>The proportion of self employed status in a population.</t>
+          <t>A self employed status population statistic that is the proportion of people that have self employed status in the population.</t>
         </is>
       </c>
       <c r="D787" t="inlineStr">
@@ -38770,7 +38770,7 @@
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>The percentage of sexual orientation in a population.</t>
+          <t>A sexual orientation population statistic that is the percentage of people that are sexual orientation in the population.</t>
         </is>
       </c>
       <c r="D789" t="inlineStr">
@@ -38821,7 +38821,7 @@
       </c>
       <c r="C790" t="inlineStr">
         <is>
-          <t>The proportion of sexual orientation in a population.</t>
+          <t>A sexual orientation population statistic that is the proportion of people that are sexual orientation in the population.</t>
         </is>
       </c>
       <c r="D790" t="inlineStr">
@@ -38923,7 +38923,7 @@
       </c>
       <c r="C792" t="inlineStr">
         <is>
-          <t>The percentage of sibling in a population.</t>
+          <t>A sibling population statistic that is the percentage of people that have a sibling in the population.</t>
         </is>
       </c>
       <c r="D792" t="inlineStr">
@@ -38974,7 +38974,7 @@
       </c>
       <c r="C793" t="inlineStr">
         <is>
-          <t>The proportion of sibling in a population.</t>
+          <t>A sibling population statistic that is the proportion of people that have a sibling in the population.</t>
         </is>
       </c>
       <c r="D793" t="inlineStr">
@@ -39076,7 +39076,7 @@
       </c>
       <c r="C795" t="inlineStr">
         <is>
-          <t>The percentage of single in a population.</t>
+          <t>A single population statistic that is the percentage of people that are single in the population.</t>
         </is>
       </c>
       <c r="D795" t="inlineStr">
@@ -39127,7 +39127,7 @@
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>The proportion of single in a population.</t>
+          <t>A single population statistic that is the proportion of people that are single in the population.</t>
         </is>
       </c>
       <c r="D796" t="inlineStr">
@@ -39229,7 +39229,7 @@
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>The percentage of socioeconomic status category in a population.</t>
+          <t>A socioeconomic status category population statistic that is the percentage of people that have a socioeconomic status category in the population.</t>
         </is>
       </c>
       <c r="D798" t="inlineStr">
@@ -39280,7 +39280,7 @@
       </c>
       <c r="C799" t="inlineStr">
         <is>
-          <t>The proportion of socioeconomic status category in a population.</t>
+          <t>A socioeconomic status category population statistic that is the proportion of people that have a socioeconomic status category in the population.</t>
         </is>
       </c>
       <c r="D799" t="inlineStr">
@@ -39382,7 +39382,7 @@
       </c>
       <c r="C801" t="inlineStr">
         <is>
-          <t>The mean of socioeconomic status score in a population.</t>
+          <t>A socioeconomic status score population statistic that is the mean value of socioeconomic status score in the population.</t>
         </is>
       </c>
       <c r="D801" t="inlineStr">
@@ -39433,7 +39433,7 @@
       </c>
       <c r="C802" t="inlineStr">
         <is>
-          <t>The minimum of socioeconomic status score in a population.</t>
+          <t>A socioeconomic status score population statistic that is the minimum value of socioeconomic status score in the population.</t>
         </is>
       </c>
       <c r="D802" t="inlineStr">
@@ -39484,7 +39484,7 @@
       </c>
       <c r="C803" t="inlineStr">
         <is>
-          <t>The maximum of socioeconomic status score in a population.</t>
+          <t>A socioeconomic status score population statistic that is the maximum value of socioeconomic status score in the population.</t>
         </is>
       </c>
       <c r="D803" t="inlineStr">
@@ -39535,7 +39535,7 @@
       </c>
       <c r="C804" t="inlineStr">
         <is>
-          <t>The median of socioeconomic status score in a population.</t>
+          <t>A socioeconomic status score population statistic that is the median value of socioeconomic status score in the population.</t>
         </is>
       </c>
       <c r="D804" t="inlineStr">
@@ -39637,7 +39637,7 @@
       </c>
       <c r="C806" t="inlineStr">
         <is>
-          <t>The percentage of stay at home parent or guardian status in a population.</t>
+          <t>A stay at home parent or guardian status population statistic that is the percentage of people that have stay at home parent or guardian status in the population.</t>
         </is>
       </c>
       <c r="D806" t="inlineStr">
@@ -39688,7 +39688,7 @@
       </c>
       <c r="C807" t="inlineStr">
         <is>
-          <t>The proportion of stay at home parent or guardian status in a population.</t>
+          <t>A stay at home parent or guardian status population statistic that is the proportion of people that have stay at home parent or guardian status in the population.</t>
         </is>
       </c>
       <c r="D807" t="inlineStr">
@@ -39790,7 +39790,7 @@
       </c>
       <c r="C809" t="inlineStr">
         <is>
-          <t>The percentage of step-parent in a population.</t>
+          <t>A step-parent population statistic that is the percentage of people that are a step-parent in the population.</t>
         </is>
       </c>
       <c r="D809" t="inlineStr">
@@ -39841,7 +39841,7 @@
       </c>
       <c r="C810" t="inlineStr">
         <is>
-          <t>The proportion of step-parent in a population.</t>
+          <t>A step-parent population statistic that is the proportion of people that are a step-parent in the population.</t>
         </is>
       </c>
       <c r="D810" t="inlineStr">
@@ -39943,7 +39943,7 @@
       </c>
       <c r="C812" t="inlineStr">
         <is>
-          <t>The percentage of step-sibling in a population.</t>
+          <t>A step-sibling population statistic that is the percentage of people that are a step-sibling in the population.</t>
         </is>
       </c>
       <c r="D812" t="inlineStr">
@@ -39994,7 +39994,7 @@
       </c>
       <c r="C813" t="inlineStr">
         <is>
-          <t>The proportion of step-sibling in a population.</t>
+          <t>A step-sibling population statistic that is the proportion of people that are a step-sibling in the population.</t>
         </is>
       </c>
       <c r="D813" t="inlineStr">
@@ -40096,7 +40096,7 @@
       </c>
       <c r="C815" t="inlineStr">
         <is>
-          <t>The percentage of stepbrother in a population.</t>
+          <t>A stepbrother population statistic that is the percentage of people that are a stepbrother in the population.</t>
         </is>
       </c>
       <c r="D815" t="inlineStr">
@@ -40147,7 +40147,7 @@
       </c>
       <c r="C816" t="inlineStr">
         <is>
-          <t>The proportion of stepbrother in a population.</t>
+          <t>A stepbrother population statistic that is the proportion of people that are a stepbrother in the population.</t>
         </is>
       </c>
       <c r="D816" t="inlineStr">
@@ -40249,7 +40249,7 @@
       </c>
       <c r="C818" t="inlineStr">
         <is>
-          <t>The percentage of stepchild in a population.</t>
+          <t>A stepchild population statistic that is the percentage of people that are a stepchild in the population.</t>
         </is>
       </c>
       <c r="D818" t="inlineStr">
@@ -40300,7 +40300,7 @@
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>The proportion of stepchild in a population.</t>
+          <t>A stepchild population statistic that is the proportion of people that are a stepchild in the population.</t>
         </is>
       </c>
       <c r="D819" t="inlineStr">
@@ -40402,7 +40402,7 @@
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>The percentage of stepdaughter in a population.</t>
+          <t>A stepdaughter population statistic that is the percentage of people that are a stepdaughter in the population.</t>
         </is>
       </c>
       <c r="D821" t="inlineStr">
@@ -40453,7 +40453,7 @@
       </c>
       <c r="C822" t="inlineStr">
         <is>
-          <t>The proportion of stepdaughter in a population.</t>
+          <t>A stepdaughter population statistic that is the proportion of people that are a stepdaughter in the population.</t>
         </is>
       </c>
       <c r="D822" t="inlineStr">
@@ -40555,7 +40555,7 @@
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>The percentage of stepfather in a population.</t>
+          <t>A stepfather population statistic that is the percentage of people that are a stepfather in the population.</t>
         </is>
       </c>
       <c r="D824" t="inlineStr">
@@ -40606,7 +40606,7 @@
       </c>
       <c r="C825" t="inlineStr">
         <is>
-          <t>The proportion of stepfather in a population.</t>
+          <t>A stepfather population statistic that is the proportion of people that are a stepfather in the population.</t>
         </is>
       </c>
       <c r="D825" t="inlineStr">
@@ -40708,7 +40708,7 @@
       </c>
       <c r="C827" t="inlineStr">
         <is>
-          <t>The percentage of stepmother in a population.</t>
+          <t>A stepmother population statistic that is the percentage of people that are a stepmother in the population.</t>
         </is>
       </c>
       <c r="D827" t="inlineStr">
@@ -40759,7 +40759,7 @@
       </c>
       <c r="C828" t="inlineStr">
         <is>
-          <t>The proportion of stepmother in a population.</t>
+          <t>A stepmother population statistic that is the proportion of people that are a stepmother in the population.</t>
         </is>
       </c>
       <c r="D828" t="inlineStr">
@@ -40861,7 +40861,7 @@
       </c>
       <c r="C830" t="inlineStr">
         <is>
-          <t>The percentage of stepsister in a population.</t>
+          <t>A stepsister population statistic that is the percentage of people that are a stepsister in the population.</t>
         </is>
       </c>
       <c r="D830" t="inlineStr">
@@ -40912,7 +40912,7 @@
       </c>
       <c r="C831" t="inlineStr">
         <is>
-          <t>The proportion of stepsister in a population.</t>
+          <t>A stepsister population statistic that is the proportion of people that are a stepsister in the population.</t>
         </is>
       </c>
       <c r="D831" t="inlineStr">
@@ -41014,7 +41014,7 @@
       </c>
       <c r="C833" t="inlineStr">
         <is>
-          <t>The percentage of stepson in a population.</t>
+          <t>A stepson population statistic that is the percentage of people that are a stepson in the population.</t>
         </is>
       </c>
       <c r="D833" t="inlineStr">
@@ -41065,7 +41065,7 @@
       </c>
       <c r="C834" t="inlineStr">
         <is>
-          <t>The proportion of stepson in a population.</t>
+          <t>A stepson population statistic that is the proportion of people that are a stepson in the population.</t>
         </is>
       </c>
       <c r="D834" t="inlineStr">
@@ -41167,7 +41167,7 @@
       </c>
       <c r="C836" t="inlineStr">
         <is>
-          <t>The percentage of student or trainee role in a population.</t>
+          <t>A student or trainee role population statistic that is the percentage of people that have a student or trainee role in the population.</t>
         </is>
       </c>
       <c r="D836" t="inlineStr">
@@ -41218,7 +41218,7 @@
       </c>
       <c r="C837" t="inlineStr">
         <is>
-          <t>The proportion of student or trainee role in a population.</t>
+          <t>A student or trainee role population statistic that is the proportion of people that have a student or trainee role in the population.</t>
         </is>
       </c>
       <c r="D837" t="inlineStr">
@@ -41320,7 +41320,7 @@
       </c>
       <c r="C839" t="inlineStr">
         <is>
-          <t>The percentage of teenager in a population.</t>
+          <t>A teenager population statistic that is the percentage of people that are a teenager in the population.</t>
         </is>
       </c>
       <c r="D839" t="inlineStr">
@@ -41371,7 +41371,7 @@
       </c>
       <c r="C840" t="inlineStr">
         <is>
-          <t>The proportion of teenager in a population.</t>
+          <t>A teenager population statistic that is the proportion of people that are a teenager in the population.</t>
         </is>
       </c>
       <c r="D840" t="inlineStr">
@@ -41473,7 +41473,7 @@
       </c>
       <c r="C842" t="inlineStr">
         <is>
-          <t>The percentage of transgender in a population.</t>
+          <t>A transgender population statistic that is the percentage of people that are transgender in the population.</t>
         </is>
       </c>
       <c r="D842" t="inlineStr">
@@ -41524,7 +41524,7 @@
       </c>
       <c r="C843" t="inlineStr">
         <is>
-          <t>The proportion of transgender in a population.</t>
+          <t>A transgender population statistic that is the proportion of people that are transgender in the population.</t>
         </is>
       </c>
       <c r="D843" t="inlineStr">
@@ -41626,7 +41626,7 @@
       </c>
       <c r="C845" t="inlineStr">
         <is>
-          <t>The percentage of twin in a population.</t>
+          <t>A twin population statistic that is the percentage of people that are a twin in the population.</t>
         </is>
       </c>
       <c r="D845" t="inlineStr">
@@ -41677,7 +41677,7 @@
       </c>
       <c r="C846" t="inlineStr">
         <is>
-          <t>The proportion of twin in a population.</t>
+          <t>A twin population statistic that is the proportion of people that are a twin in the population.</t>
         </is>
       </c>
       <c r="D846" t="inlineStr">
@@ -41779,7 +41779,7 @@
       </c>
       <c r="C848" t="inlineStr">
         <is>
-          <t>The percentage of unawareness of a behaviour in a population.</t>
+          <t>A unawareness of a behaviour population statistic that is the percentage of people that have a unawareness of a behaviour in the population.</t>
         </is>
       </c>
       <c r="D848" t="inlineStr">
@@ -41830,7 +41830,7 @@
       </c>
       <c r="C849" t="inlineStr">
         <is>
-          <t>The proportion of unawareness of a behaviour in a population.</t>
+          <t>A unawareness of a behaviour population statistic that is the proportion of people that have a unawareness of a behaviour in the population.</t>
         </is>
       </c>
       <c r="D849" t="inlineStr">
@@ -41932,7 +41932,7 @@
       </c>
       <c r="C851" t="inlineStr">
         <is>
-          <t>The percentage of uncle in a population.</t>
+          <t>A uncle population statistic that is the percentage of people that are a uncle in the population.</t>
         </is>
       </c>
       <c r="D851" t="inlineStr">
@@ -41983,7 +41983,7 @@
       </c>
       <c r="C852" t="inlineStr">
         <is>
-          <t>The proportion of uncle in a population.</t>
+          <t>A uncle population statistic that is the proportion of people that are a uncle in the population.</t>
         </is>
       </c>
       <c r="D852" t="inlineStr">
@@ -42085,7 +42085,7 @@
       </c>
       <c r="C854" t="inlineStr">
         <is>
-          <t>The percentage of undecidedness about enacting a behaviour in a population.</t>
+          <t>A undecidedness about enacting a behaviour population statistic that is the percentage of people that have a undecidedness about enacting a behaviour in the population.</t>
         </is>
       </c>
       <c r="D854" t="inlineStr">
@@ -42136,7 +42136,7 @@
       </c>
       <c r="C855" t="inlineStr">
         <is>
-          <t>The proportion of undecidedness about enacting a behaviour in a population.</t>
+          <t>A undecidedness about enacting a behaviour population statistic that is the proportion of people that have a undecidedness about enacting a behaviour in the population.</t>
         </is>
       </c>
       <c r="D855" t="inlineStr">
@@ -42238,7 +42238,7 @@
       </c>
       <c r="C857" t="inlineStr">
         <is>
-          <t>The percentage of undergraduate student role in a population.</t>
+          <t>A undergraduate student role population statistic that is the percentage of people that have a undergraduate student role in the population.</t>
         </is>
       </c>
       <c r="D857" t="inlineStr">
@@ -42289,7 +42289,7 @@
       </c>
       <c r="C858" t="inlineStr">
         <is>
-          <t>The proportion of undergraduate student role in a population.</t>
+          <t>A undergraduate student role population statistic that is the proportion of people that have a undergraduate student role in the population.</t>
         </is>
       </c>
       <c r="D858" t="inlineStr">
@@ -42391,7 +42391,7 @@
       </c>
       <c r="C860" t="inlineStr">
         <is>
-          <t>The percentage of unemployed in a population.</t>
+          <t>A unemployed population statistic that is the percentage of people that are unemployed in the population.</t>
         </is>
       </c>
       <c r="D860" t="inlineStr">
@@ -42442,7 +42442,7 @@
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>The proportion of unemployed in a population.</t>
+          <t>A unemployed population statistic that is the proportion of people that are unemployed in the population.</t>
         </is>
       </c>
       <c r="D861" t="inlineStr">
@@ -42544,7 +42544,7 @@
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>The percentage of unpaid carer for an adult status in a population.</t>
+          <t>A unpaid carer for an adult status population statistic that is the percentage of people that have unpaid carer for an adult status in the population.</t>
         </is>
       </c>
       <c r="D863" t="inlineStr">
@@ -42595,7 +42595,7 @@
       </c>
       <c r="C864" t="inlineStr">
         <is>
-          <t>The proportion of unpaid carer for an adult status in a population.</t>
+          <t>A unpaid carer for an adult status population statistic that is the proportion of people that have unpaid carer for an adult status in the population.</t>
         </is>
       </c>
       <c r="D864" t="inlineStr">
@@ -42697,7 +42697,7 @@
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>The mean of value of valuable material resource owned in a population.</t>
+          <t>A value of valuable material resource owned population statistic that is the mean value of value of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D866" t="inlineStr">
@@ -42748,7 +42748,7 @@
       </c>
       <c r="C867" t="inlineStr">
         <is>
-          <t>The minimum of value of valuable material resource owned in a population.</t>
+          <t>A value of valuable material resource owned population statistic that is the minimum value of value of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D867" t="inlineStr">
@@ -42799,7 +42799,7 @@
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>The maximum of value of valuable material resource owned in a population.</t>
+          <t>A value of valuable material resource owned population statistic that is the maximum value of value of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D868" t="inlineStr">
@@ -42850,7 +42850,7 @@
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>The median of value of valuable material resource owned in a population.</t>
+          <t>A value of valuable material resource owned population statistic that is the median value of value of valuable material resource owned in the population.</t>
         </is>
       </c>
       <c r="D869" t="inlineStr">
@@ -42952,7 +42952,7 @@
       </c>
       <c r="C871" t="inlineStr">
         <is>
-          <t>The percentage of vocational training student or trainee role in a population.</t>
+          <t>A vocational training student or trainee role population statistic that is the percentage of people that have a vocational training student or trainee role in the population.</t>
         </is>
       </c>
       <c r="D871" t="inlineStr">
@@ -43003,7 +43003,7 @@
       </c>
       <c r="C872" t="inlineStr">
         <is>
-          <t>The proportion of vocational training student or trainee role in a population.</t>
+          <t>A vocational training student or trainee role population statistic that is the proportion of people that have a vocational training student or trainee role in the population.</t>
         </is>
       </c>
       <c r="D872" t="inlineStr">
@@ -43105,7 +43105,7 @@
       </c>
       <c r="C874" t="inlineStr">
         <is>
-          <t>The percentage of voluntary worker status in a population.</t>
+          <t>A voluntary worker status population statistic that is the percentage of people that have voluntary worker status in the population.</t>
         </is>
       </c>
       <c r="D874" t="inlineStr">
@@ -43156,7 +43156,7 @@
       </c>
       <c r="C875" t="inlineStr">
         <is>
-          <t>The proportion of voluntary worker status in a population.</t>
+          <t>A voluntary worker status population statistic that is the proportion of people that have voluntary worker status in the population.</t>
         </is>
       </c>
       <c r="D875" t="inlineStr">
@@ -43258,7 +43258,7 @@
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>The percentage of widowed in a population.</t>
+          <t>A widowed population statistic that is the percentage of people that are widowed in the population.</t>
         </is>
       </c>
       <c r="D877" t="inlineStr">
@@ -43309,7 +43309,7 @@
       </c>
       <c r="C878" t="inlineStr">
         <is>
-          <t>The proportion of widowed in a population.</t>
+          <t>A widowed population statistic that is the proportion of people that are widowed in the population.</t>
         </is>
       </c>
       <c r="D878" t="inlineStr">

</xml_diff>